<commit_message>
Updated template file to avoid trailing "_" in site code
</commit_message>
<xml_diff>
--- a/sfnform/static/sfnform/media/sapfluxnet_metadata_template.xlsx
+++ b/sfnform/static/sfnform/media/sapfluxnet_metadata_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10470" windowHeight="8085" tabRatio="796"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10470" windowHeight="8085" tabRatio="796" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="site_md" sheetId="1" r:id="rId1"/>
@@ -5259,7 +5259,9 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.7109375" defaultRowHeight="12.75"/>
   <cols>
@@ -5563,8 +5565,8 @@
         <v>1037</v>
       </c>
       <c r="D22" s="94" t="str">
-        <f>IFERROR(UPPER(LEFT(site_md!D4,3)) &amp; "_" &amp; UPPER(LEFT(site_md!D3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!D2,3)) &amp; IF(ISBLANK(stand_md!D4),"","_") &amp; UPPER(LEFT(stand_md!D4,3)), "")</f>
-        <v>__</v>
+        <f>IFERROR(UPPER(LEFT(site_md!D4,3)) &amp; "_" &amp; UPPER(LEFT(site_md!D3,3)) &amp; IF(ISBLANK(stand_md!D2),"","_") &amp; UPPER(LEFT(stand_md!D2,3)) &amp; IF(ISBLANK(stand_md!D4),"","_") &amp; UPPER(LEFT(stand_md!D4,3)), "")</f>
+        <v>_</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -5618,7 +5620,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Site name" prompt="Please fill in the site name" sqref="D3">
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Site name" prompt="Please fill in the site name (letters and numbers only)" sqref="D3">
       <formula1>250</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Coordinates error" error="Entered value is not correct, please ensure that is a number and it is in_x000a_decimal format (use the longitude/latitude converter in the &quot;site_dic&quot;_x000a_sheet if you need help with converting degrees, minutes and seconds_x000a_to decimal format)" promptTitle="Coordinates" prompt="Please introduce coordinates in decimal format (See &quot;site_dic&quot; sheet for a longitude/latitude converter)" sqref="D13">
@@ -6788,7 +6790,9 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
@@ -7044,9 +7048,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Soil texture" prompt="Please specify a value from the list if qualitative assesment of soil texture was made. In case of quantitiative assesment, please fill the fileds below with the percentages." sqref="D13">
       <formula1>soil_texture_2</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Stand treatment" prompt="Please fill in the treatment applied to stand. Leave blank if no treatment was applied." sqref="D4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Stand treatment" prompt="Please fill in the treatment applied to stand. Leave blank if no treatment was applied._x000a_Letters and numbers only." sqref="D4"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Remarks" prompt="Please add any information relevant to stand-specific peculiarities that may not have been adequately captured by the stand-level metadata." sqref="D17"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Stand code" prompt="Please fill if more than one stand per site is provided._x000a_Leave blank if only one stand per site is provided." sqref="D2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Stand code" prompt="Please fill if more than one stand per site is provided._x000a_Leave blank if only one stand per site is provided._x000a_Letters and numbers only." sqref="D2"/>
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Age error" error="Value is not a number or it is not greater than 0" sqref="D5">
       <formula1>0</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Fixed automatic plant code to reflect stand name and treatment
</commit_message>
<xml_diff>
--- a/sfnform/static/sfnform/media/sapfluxnet_metadata_template.xlsx
+++ b/sfnform/static/sfnform/media/sapfluxnet_metadata_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10470" windowHeight="8085" tabRatio="796" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10470" windowHeight="8085" tabRatio="796"/>
   </bookViews>
   <sheets>
     <sheet name="site_md" sheetId="1" r:id="rId1"/>
@@ -5259,9 +5259,7 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.7109375" defaultRowHeight="12.75"/>
   <cols>
@@ -6790,9 +6788,7 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
@@ -10475,403 +10471,403 @@
         <v>1037</v>
       </c>
       <c r="D25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!D$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!D$3,1) &amp; RIGHT(plant_md!D$3,LEN(plant_md!D$3)-FIND(" ",plant_md!D$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!B3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!B3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!D$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!D$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!D2),"","_") &amp; UPPER(LEFT(stand_md!D2,3)) &amp; IF(ISBLANK(stand_md!D4),"","_") &amp; UPPER(LEFT(stand_md!D4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!D$3,1) &amp; RIGHT(plant_md!D$3,LEN(plant_md!D$3)-FIND(" ",plant_md!D$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!B3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!B3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!D$1,"")</f>
         <v/>
       </c>
       <c r="E25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!E$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!E$3,1) &amp; RIGHT(plant_md!E$3,LEN(plant_md!E$3)-FIND(" ",plant_md!E$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!C3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!C3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!E$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!E$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!E2),"","_") &amp; UPPER(LEFT(stand_md!E2,3)) &amp; IF(ISBLANK(stand_md!E4),"","_") &amp; UPPER(LEFT(stand_md!E4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!E$3,1) &amp; RIGHT(plant_md!E$3,LEN(plant_md!E$3)-FIND(" ",plant_md!E$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!C3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!C3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!E$1,"")</f>
         <v/>
       </c>
       <c r="F25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!F$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!F$3,1) &amp; RIGHT(plant_md!F$3,LEN(plant_md!F$3)-FIND(" ",plant_md!F$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!D3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!D3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!F$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!F$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!F2),"","_") &amp; UPPER(LEFT(stand_md!F2,3)) &amp; IF(ISBLANK(stand_md!F4),"","_") &amp; UPPER(LEFT(stand_md!F4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!F$3,1) &amp; RIGHT(plant_md!F$3,LEN(plant_md!F$3)-FIND(" ",plant_md!F$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!D3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!D3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!F$1,"")</f>
         <v/>
       </c>
       <c r="G25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!G$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!G$3,1) &amp; RIGHT(plant_md!G$3,LEN(plant_md!G$3)-FIND(" ",plant_md!G$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!E3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!E3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!G$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!G$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!G2),"","_") &amp; UPPER(LEFT(stand_md!G2,3)) &amp; IF(ISBLANK(stand_md!G4),"","_") &amp; UPPER(LEFT(stand_md!G4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!G$3,1) &amp; RIGHT(plant_md!G$3,LEN(plant_md!G$3)-FIND(" ",plant_md!G$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!E3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!E3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!G$1,"")</f>
         <v/>
       </c>
       <c r="H25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!H$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!H$3,1) &amp; RIGHT(plant_md!H$3,LEN(plant_md!H$3)-FIND(" ",plant_md!H$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!F3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!F3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!H$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!H$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!H2),"","_") &amp; UPPER(LEFT(stand_md!H2,3)) &amp; IF(ISBLANK(stand_md!H4),"","_") &amp; UPPER(LEFT(stand_md!H4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!H$3,1) &amp; RIGHT(plant_md!H$3,LEN(plant_md!H$3)-FIND(" ",plant_md!H$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!F3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!F3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!H$1,"")</f>
         <v/>
       </c>
       <c r="I25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!I$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!I$3,1) &amp; RIGHT(plant_md!I$3,LEN(plant_md!I$3)-FIND(" ",plant_md!I$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!G3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!G3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!I$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!I$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!I2),"","_") &amp; UPPER(LEFT(stand_md!I2,3)) &amp; IF(ISBLANK(stand_md!I4),"","_") &amp; UPPER(LEFT(stand_md!I4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!I$3,1) &amp; RIGHT(plant_md!I$3,LEN(plant_md!I$3)-FIND(" ",plant_md!I$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!G3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!G3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!I$1,"")</f>
         <v/>
       </c>
       <c r="J25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!J$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!J$3,1) &amp; RIGHT(plant_md!J$3,LEN(plant_md!J$3)-FIND(" ",plant_md!J$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!H3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!H3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!J$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!J$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!J2),"","_") &amp; UPPER(LEFT(stand_md!J2,3)) &amp; IF(ISBLANK(stand_md!J4),"","_") &amp; UPPER(LEFT(stand_md!J4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!J$3,1) &amp; RIGHT(plant_md!J$3,LEN(plant_md!J$3)-FIND(" ",plant_md!J$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!H3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!H3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!J$1,"")</f>
         <v/>
       </c>
       <c r="K25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!K$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!K$3,1) &amp; RIGHT(plant_md!K$3,LEN(plant_md!K$3)-FIND(" ",plant_md!K$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!I3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!I3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!K$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!K$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!K2),"","_") &amp; UPPER(LEFT(stand_md!K2,3)) &amp; IF(ISBLANK(stand_md!K4),"","_") &amp; UPPER(LEFT(stand_md!K4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!K$3,1) &amp; RIGHT(plant_md!K$3,LEN(plant_md!K$3)-FIND(" ",plant_md!K$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!I3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!I3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!K$1,"")</f>
         <v/>
       </c>
       <c r="L25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!L$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!L$3,1) &amp; RIGHT(plant_md!L$3,LEN(plant_md!L$3)-FIND(" ",plant_md!L$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!J3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!J3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!L$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!L$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!L2),"","_") &amp; UPPER(LEFT(stand_md!L2,3)) &amp; IF(ISBLANK(stand_md!L4),"","_") &amp; UPPER(LEFT(stand_md!L4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!L$3,1) &amp; RIGHT(plant_md!L$3,LEN(plant_md!L$3)-FIND(" ",plant_md!L$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!J3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!J3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!L$1,"")</f>
         <v/>
       </c>
       <c r="M25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!M$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!M$3,1) &amp; RIGHT(plant_md!M$3,LEN(plant_md!M$3)-FIND(" ",plant_md!M$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!K3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!K3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!M$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!M$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!M2),"","_") &amp; UPPER(LEFT(stand_md!M2,3)) &amp; IF(ISBLANK(stand_md!M4),"","_") &amp; UPPER(LEFT(stand_md!M4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!M$3,1) &amp; RIGHT(plant_md!M$3,LEN(plant_md!M$3)-FIND(" ",plant_md!M$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!K3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!K3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!M$1,"")</f>
         <v/>
       </c>
       <c r="N25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!N$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!N$3,1) &amp; RIGHT(plant_md!N$3,LEN(plant_md!N$3)-FIND(" ",plant_md!N$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!L3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!L3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!N$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!N$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!N2),"","_") &amp; UPPER(LEFT(stand_md!N2,3)) &amp; IF(ISBLANK(stand_md!N4),"","_") &amp; UPPER(LEFT(stand_md!N4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!N$3,1) &amp; RIGHT(plant_md!N$3,LEN(plant_md!N$3)-FIND(" ",plant_md!N$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!L3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!L3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!N$1,"")</f>
         <v/>
       </c>
       <c r="O25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!O$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!O$3,1) &amp; RIGHT(plant_md!O$3,LEN(plant_md!O$3)-FIND(" ",plant_md!O$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!M3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!M3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!O$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!O$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!O2),"","_") &amp; UPPER(LEFT(stand_md!O2,3)) &amp; IF(ISBLANK(stand_md!O4),"","_") &amp; UPPER(LEFT(stand_md!O4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!O$3,1) &amp; RIGHT(plant_md!O$3,LEN(plant_md!O$3)-FIND(" ",plant_md!O$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!M3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!M3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!O$1,"")</f>
         <v/>
       </c>
       <c r="P25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!P$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!P$3,1) &amp; RIGHT(plant_md!P$3,LEN(plant_md!P$3)-FIND(" ",plant_md!P$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!N3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!N3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!P$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!P$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!P2),"","_") &amp; UPPER(LEFT(stand_md!P2,3)) &amp; IF(ISBLANK(stand_md!P4),"","_") &amp; UPPER(LEFT(stand_md!P4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!P$3,1) &amp; RIGHT(plant_md!P$3,LEN(plant_md!P$3)-FIND(" ",plant_md!P$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!N3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!N3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!P$1,"")</f>
         <v/>
       </c>
       <c r="Q25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!Q$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Q$3,1) &amp; RIGHT(plant_md!Q$3,LEN(plant_md!Q$3)-FIND(" ",plant_md!Q$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!O3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!O3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Q$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!Q$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!Q2),"","_") &amp; UPPER(LEFT(stand_md!Q2,3)) &amp; IF(ISBLANK(stand_md!Q4),"","_") &amp; UPPER(LEFT(stand_md!Q4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Q$3,1) &amp; RIGHT(plant_md!Q$3,LEN(plant_md!Q$3)-FIND(" ",plant_md!Q$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!O3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!O3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Q$1,"")</f>
         <v/>
       </c>
       <c r="R25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!R$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!R$3,1) &amp; RIGHT(plant_md!R$3,LEN(plant_md!R$3)-FIND(" ",plant_md!R$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!P3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!P3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!R$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!R$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!R2),"","_") &amp; UPPER(LEFT(stand_md!R2,3)) &amp; IF(ISBLANK(stand_md!R4),"","_") &amp; UPPER(LEFT(stand_md!R4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!R$3,1) &amp; RIGHT(plant_md!R$3,LEN(plant_md!R$3)-FIND(" ",plant_md!R$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!P3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!P3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!R$1,"")</f>
         <v/>
       </c>
       <c r="S25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!S$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!S$3,1) &amp; RIGHT(plant_md!S$3,LEN(plant_md!S$3)-FIND(" ",plant_md!S$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Q3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Q3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!S$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!S$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!S2),"","_") &amp; UPPER(LEFT(stand_md!S2,3)) &amp; IF(ISBLANK(stand_md!S4),"","_") &amp; UPPER(LEFT(stand_md!S4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!S$3,1) &amp; RIGHT(plant_md!S$3,LEN(plant_md!S$3)-FIND(" ",plant_md!S$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Q3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Q3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!S$1,"")</f>
         <v/>
       </c>
       <c r="T25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!T$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!T$3,1) &amp; RIGHT(plant_md!T$3,LEN(plant_md!T$3)-FIND(" ",plant_md!T$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!R3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!R3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!T$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!T$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!T2),"","_") &amp; UPPER(LEFT(stand_md!T2,3)) &amp; IF(ISBLANK(stand_md!T4),"","_") &amp; UPPER(LEFT(stand_md!T4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!T$3,1) &amp; RIGHT(plant_md!T$3,LEN(plant_md!T$3)-FIND(" ",plant_md!T$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!R3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!R3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!T$1,"")</f>
         <v/>
       </c>
       <c r="U25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!U$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!U$3,1) &amp; RIGHT(plant_md!U$3,LEN(plant_md!U$3)-FIND(" ",plant_md!U$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!S3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!S3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!U$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!U$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!U2),"","_") &amp; UPPER(LEFT(stand_md!U2,3)) &amp; IF(ISBLANK(stand_md!U4),"","_") &amp; UPPER(LEFT(stand_md!U4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!U$3,1) &amp; RIGHT(plant_md!U$3,LEN(plant_md!U$3)-FIND(" ",plant_md!U$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!S3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!S3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!U$1,"")</f>
         <v/>
       </c>
       <c r="V25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!V$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!V$3,1) &amp; RIGHT(plant_md!V$3,LEN(plant_md!V$3)-FIND(" ",plant_md!V$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!T3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!T3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!V$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!V$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!V2),"","_") &amp; UPPER(LEFT(stand_md!V2,3)) &amp; IF(ISBLANK(stand_md!V4),"","_") &amp; UPPER(LEFT(stand_md!V4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!V$3,1) &amp; RIGHT(plant_md!V$3,LEN(plant_md!V$3)-FIND(" ",plant_md!V$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!T3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!T3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!V$1,"")</f>
         <v/>
       </c>
       <c r="W25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!W$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!W$3,1) &amp; RIGHT(plant_md!W$3,LEN(plant_md!W$3)-FIND(" ",plant_md!W$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!U3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!U3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!W$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!W$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!W2),"","_") &amp; UPPER(LEFT(stand_md!W2,3)) &amp; IF(ISBLANK(stand_md!W4),"","_") &amp; UPPER(LEFT(stand_md!W4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!W$3,1) &amp; RIGHT(plant_md!W$3,LEN(plant_md!W$3)-FIND(" ",plant_md!W$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!U3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!U3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!W$1,"")</f>
         <v/>
       </c>
       <c r="X25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!X$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!X$3,1) &amp; RIGHT(plant_md!X$3,LEN(plant_md!X$3)-FIND(" ",plant_md!X$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!V3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!V3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!X$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!X$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!X2),"","_") &amp; UPPER(LEFT(stand_md!X2,3)) &amp; IF(ISBLANK(stand_md!X4),"","_") &amp; UPPER(LEFT(stand_md!X4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!X$3,1) &amp; RIGHT(plant_md!X$3,LEN(plant_md!X$3)-FIND(" ",plant_md!X$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!V3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!V3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!X$1,"")</f>
         <v/>
       </c>
       <c r="Y25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!Y$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Y$3,1) &amp; RIGHT(plant_md!Y$3,LEN(plant_md!Y$3)-FIND(" ",plant_md!Y$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!W3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!W3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Y$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!Y$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!Y2),"","_") &amp; UPPER(LEFT(stand_md!Y2,3)) &amp; IF(ISBLANK(stand_md!Y4),"","_") &amp; UPPER(LEFT(stand_md!Y4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Y$3,1) &amp; RIGHT(plant_md!Y$3,LEN(plant_md!Y$3)-FIND(" ",plant_md!Y$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!W3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!W3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Y$1,"")</f>
         <v/>
       </c>
       <c r="Z25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!Z$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Z$3,1) &amp; RIGHT(plant_md!Z$3,LEN(plant_md!Z$3)-FIND(" ",plant_md!Z$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!X3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!X3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Z$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!Z$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!Z2),"","_") &amp; UPPER(LEFT(stand_md!Z2,3)) &amp; IF(ISBLANK(stand_md!Z4),"","_") &amp; UPPER(LEFT(stand_md!Z4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Z$3,1) &amp; RIGHT(plant_md!Z$3,LEN(plant_md!Z$3)-FIND(" ",plant_md!Z$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!X3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!X3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Z$1,"")</f>
         <v/>
       </c>
       <c r="AA25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AA$3,1) &amp; RIGHT(plant_md!AA$3,LEN(plant_md!AA$3)-FIND(" ",plant_md!AA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Y3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Y3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AA$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AA2),"","_") &amp; UPPER(LEFT(stand_md!AA2,3)) &amp; IF(ISBLANK(stand_md!AA4),"","_") &amp; UPPER(LEFT(stand_md!AA4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AA$3,1) &amp; RIGHT(plant_md!AA$3,LEN(plant_md!AA$3)-FIND(" ",plant_md!AA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Y3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Y3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AA$1,"")</f>
         <v/>
       </c>
       <c r="AB25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AB$3,1) &amp; RIGHT(plant_md!AB$3,LEN(plant_md!AB$3)-FIND(" ",plant_md!AB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Z3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Z3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AB$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AB2),"","_") &amp; UPPER(LEFT(stand_md!AB2,3)) &amp; IF(ISBLANK(stand_md!AB4),"","_") &amp; UPPER(LEFT(stand_md!AB4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AB$3,1) &amp; RIGHT(plant_md!AB$3,LEN(plant_md!AB$3)-FIND(" ",plant_md!AB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Z3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Z3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AB$1,"")</f>
         <v/>
       </c>
       <c r="AC25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AC$3,1) &amp; RIGHT(plant_md!AC$3,LEN(plant_md!AC$3)-FIND(" ",plant_md!AC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AC$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AC2),"","_") &amp; UPPER(LEFT(stand_md!AC2,3)) &amp; IF(ISBLANK(stand_md!AC4),"","_") &amp; UPPER(LEFT(stand_md!AC4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AC$3,1) &amp; RIGHT(plant_md!AC$3,LEN(plant_md!AC$3)-FIND(" ",plant_md!AC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AC$1,"")</f>
         <v/>
       </c>
       <c r="AD25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AD$3,1) &amp; RIGHT(plant_md!AD$3,LEN(plant_md!AD$3)-FIND(" ",plant_md!AD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AD$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AD2),"","_") &amp; UPPER(LEFT(stand_md!AD2,3)) &amp; IF(ISBLANK(stand_md!AD4),"","_") &amp; UPPER(LEFT(stand_md!AD4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AD$3,1) &amp; RIGHT(plant_md!AD$3,LEN(plant_md!AD$3)-FIND(" ",plant_md!AD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AD$1,"")</f>
         <v/>
       </c>
       <c r="AE25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AE$3,1) &amp; RIGHT(plant_md!AE$3,LEN(plant_md!AE$3)-FIND(" ",plant_md!AE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AE$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AE2),"","_") &amp; UPPER(LEFT(stand_md!AE2,3)) &amp; IF(ISBLANK(stand_md!AE4),"","_") &amp; UPPER(LEFT(stand_md!AE4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AE$3,1) &amp; RIGHT(plant_md!AE$3,LEN(plant_md!AE$3)-FIND(" ",plant_md!AE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AE$1,"")</f>
         <v/>
       </c>
       <c r="AF25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AF$3,1) &amp; RIGHT(plant_md!AF$3,LEN(plant_md!AF$3)-FIND(" ",plant_md!AF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AF$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AF2),"","_") &amp; UPPER(LEFT(stand_md!AF2,3)) &amp; IF(ISBLANK(stand_md!AF4),"","_") &amp; UPPER(LEFT(stand_md!AF4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AF$3,1) &amp; RIGHT(plant_md!AF$3,LEN(plant_md!AF$3)-FIND(" ",plant_md!AF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AF$1,"")</f>
         <v/>
       </c>
       <c r="AG25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AG$3,1) &amp; RIGHT(plant_md!AG$3,LEN(plant_md!AG$3)-FIND(" ",plant_md!AG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AG$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AG2),"","_") &amp; UPPER(LEFT(stand_md!AG2,3)) &amp; IF(ISBLANK(stand_md!AG4),"","_") &amp; UPPER(LEFT(stand_md!AG4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AG$3,1) &amp; RIGHT(plant_md!AG$3,LEN(plant_md!AG$3)-FIND(" ",plant_md!AG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AG$1,"")</f>
         <v/>
       </c>
       <c r="AH25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AH$3,1) &amp; RIGHT(plant_md!AH$3,LEN(plant_md!AH$3)-FIND(" ",plant_md!AH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AH$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AH2),"","_") &amp; UPPER(LEFT(stand_md!AH2,3)) &amp; IF(ISBLANK(stand_md!AH4),"","_") &amp; UPPER(LEFT(stand_md!AH4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AH$3,1) &amp; RIGHT(plant_md!AH$3,LEN(plant_md!AH$3)-FIND(" ",plant_md!AH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AH$1,"")</f>
         <v/>
       </c>
       <c r="AI25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AI$3,1) &amp; RIGHT(plant_md!AI$3,LEN(plant_md!AI$3)-FIND(" ",plant_md!AI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AI$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AI2),"","_") &amp; UPPER(LEFT(stand_md!AI2,3)) &amp; IF(ISBLANK(stand_md!AI4),"","_") &amp; UPPER(LEFT(stand_md!AI4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AI$3,1) &amp; RIGHT(plant_md!AI$3,LEN(plant_md!AI$3)-FIND(" ",plant_md!AI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AI$1,"")</f>
         <v/>
       </c>
       <c r="AJ25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AJ$3,1) &amp; RIGHT(plant_md!AJ$3,LEN(plant_md!AJ$3)-FIND(" ",plant_md!AJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AJ$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AJ2),"","_") &amp; UPPER(LEFT(stand_md!AJ2,3)) &amp; IF(ISBLANK(stand_md!AJ4),"","_") &amp; UPPER(LEFT(stand_md!AJ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AJ$3,1) &amp; RIGHT(plant_md!AJ$3,LEN(plant_md!AJ$3)-FIND(" ",plant_md!AJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AJ$1,"")</f>
         <v/>
       </c>
       <c r="AK25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AK$3,1) &amp; RIGHT(plant_md!AK$3,LEN(plant_md!AK$3)-FIND(" ",plant_md!AK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AK$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AK2),"","_") &amp; UPPER(LEFT(stand_md!AK2,3)) &amp; IF(ISBLANK(stand_md!AK4),"","_") &amp; UPPER(LEFT(stand_md!AK4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AK$3,1) &amp; RIGHT(plant_md!AK$3,LEN(plant_md!AK$3)-FIND(" ",plant_md!AK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AK$1,"")</f>
         <v/>
       </c>
       <c r="AL25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AL$3,1) &amp; RIGHT(plant_md!AL$3,LEN(plant_md!AL$3)-FIND(" ",plant_md!AL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AL$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AL2),"","_") &amp; UPPER(LEFT(stand_md!AL2,3)) &amp; IF(ISBLANK(stand_md!AL4),"","_") &amp; UPPER(LEFT(stand_md!AL4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AL$3,1) &amp; RIGHT(plant_md!AL$3,LEN(plant_md!AL$3)-FIND(" ",plant_md!AL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AL$1,"")</f>
         <v/>
       </c>
       <c r="AM25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AM$3,1) &amp; RIGHT(plant_md!AM$3,LEN(plant_md!AM$3)-FIND(" ",plant_md!AM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AM$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AM2),"","_") &amp; UPPER(LEFT(stand_md!AM2,3)) &amp; IF(ISBLANK(stand_md!AM4),"","_") &amp; UPPER(LEFT(stand_md!AM4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AM$3,1) &amp; RIGHT(plant_md!AM$3,LEN(plant_md!AM$3)-FIND(" ",plant_md!AM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AM$1,"")</f>
         <v/>
       </c>
       <c r="AN25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AN$3,1) &amp; RIGHT(plant_md!AN$3,LEN(plant_md!AN$3)-FIND(" ",plant_md!AN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AN$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AN2),"","_") &amp; UPPER(LEFT(stand_md!AN2,3)) &amp; IF(ISBLANK(stand_md!AN4),"","_") &amp; UPPER(LEFT(stand_md!AN4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AN$3,1) &amp; RIGHT(plant_md!AN$3,LEN(plant_md!AN$3)-FIND(" ",plant_md!AN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AN$1,"")</f>
         <v/>
       </c>
       <c r="AO25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AO$3,1) &amp; RIGHT(plant_md!AO$3,LEN(plant_md!AO$3)-FIND(" ",plant_md!AO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AO$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AO2),"","_") &amp; UPPER(LEFT(stand_md!AO2,3)) &amp; IF(ISBLANK(stand_md!AO4),"","_") &amp; UPPER(LEFT(stand_md!AO4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AO$3,1) &amp; RIGHT(plant_md!AO$3,LEN(plant_md!AO$3)-FIND(" ",plant_md!AO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AO$1,"")</f>
         <v/>
       </c>
       <c r="AP25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AP$3,1) &amp; RIGHT(plant_md!AP$3,LEN(plant_md!AP$3)-FIND(" ",plant_md!AP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AP$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AP2),"","_") &amp; UPPER(LEFT(stand_md!AP2,3)) &amp; IF(ISBLANK(stand_md!AP4),"","_") &amp; UPPER(LEFT(stand_md!AP4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AP$3,1) &amp; RIGHT(plant_md!AP$3,LEN(plant_md!AP$3)-FIND(" ",plant_md!AP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AP$1,"")</f>
         <v/>
       </c>
       <c r="AQ25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AQ$3,1) &amp; RIGHT(plant_md!AQ$3,LEN(plant_md!AQ$3)-FIND(" ",plant_md!AQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AQ$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AQ2),"","_") &amp; UPPER(LEFT(stand_md!AQ2,3)) &amp; IF(ISBLANK(stand_md!AQ4),"","_") &amp; UPPER(LEFT(stand_md!AQ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AQ$3,1) &amp; RIGHT(plant_md!AQ$3,LEN(plant_md!AQ$3)-FIND(" ",plant_md!AQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AQ$1,"")</f>
         <v/>
       </c>
       <c r="AR25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AR$3,1) &amp; RIGHT(plant_md!AR$3,LEN(plant_md!AR$3)-FIND(" ",plant_md!AR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AR$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AR2),"","_") &amp; UPPER(LEFT(stand_md!AR2,3)) &amp; IF(ISBLANK(stand_md!AR4),"","_") &amp; UPPER(LEFT(stand_md!AR4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AR$3,1) &amp; RIGHT(plant_md!AR$3,LEN(plant_md!AR$3)-FIND(" ",plant_md!AR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AR$1,"")</f>
         <v/>
       </c>
       <c r="AS25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AS$3,1) &amp; RIGHT(plant_md!AS$3,LEN(plant_md!AS$3)-FIND(" ",plant_md!AS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AS$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AS2),"","_") &amp; UPPER(LEFT(stand_md!AS2,3)) &amp; IF(ISBLANK(stand_md!AS4),"","_") &amp; UPPER(LEFT(stand_md!AS4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AS$3,1) &amp; RIGHT(plant_md!AS$3,LEN(plant_md!AS$3)-FIND(" ",plant_md!AS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AS$1,"")</f>
         <v/>
       </c>
       <c r="AT25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AT$3,1) &amp; RIGHT(plant_md!AT$3,LEN(plant_md!AT$3)-FIND(" ",plant_md!AT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AT$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AT2),"","_") &amp; UPPER(LEFT(stand_md!AT2,3)) &amp; IF(ISBLANK(stand_md!AT4),"","_") &amp; UPPER(LEFT(stand_md!AT4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AT$3,1) &amp; RIGHT(plant_md!AT$3,LEN(plant_md!AT$3)-FIND(" ",plant_md!AT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AT$1,"")</f>
         <v/>
       </c>
       <c r="AU25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AU$3,1) &amp; RIGHT(plant_md!AU$3,LEN(plant_md!AU$3)-FIND(" ",plant_md!AU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AU$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AU2),"","_") &amp; UPPER(LEFT(stand_md!AU2,3)) &amp; IF(ISBLANK(stand_md!AU4),"","_") &amp; UPPER(LEFT(stand_md!AU4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AU$3,1) &amp; RIGHT(plant_md!AU$3,LEN(plant_md!AU$3)-FIND(" ",plant_md!AU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AU$1,"")</f>
         <v/>
       </c>
       <c r="AV25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AV$3,1) &amp; RIGHT(plant_md!AV$3,LEN(plant_md!AV$3)-FIND(" ",plant_md!AV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AV$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AV2),"","_") &amp; UPPER(LEFT(stand_md!AV2,3)) &amp; IF(ISBLANK(stand_md!AV4),"","_") &amp; UPPER(LEFT(stand_md!AV4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AV$3,1) &amp; RIGHT(plant_md!AV$3,LEN(plant_md!AV$3)-FIND(" ",plant_md!AV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AV$1,"")</f>
         <v/>
       </c>
       <c r="AW25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AW$3,1) &amp; RIGHT(plant_md!AW$3,LEN(plant_md!AW$3)-FIND(" ",plant_md!AW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AW$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AW2),"","_") &amp; UPPER(LEFT(stand_md!AW2,3)) &amp; IF(ISBLANK(stand_md!AW4),"","_") &amp; UPPER(LEFT(stand_md!AW4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AW$3,1) &amp; RIGHT(plant_md!AW$3,LEN(plant_md!AW$3)-FIND(" ",plant_md!AW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AW$1,"")</f>
         <v/>
       </c>
       <c r="AX25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AX$3,1) &amp; RIGHT(plant_md!AX$3,LEN(plant_md!AX$3)-FIND(" ",plant_md!AX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AX$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AX2),"","_") &amp; UPPER(LEFT(stand_md!AX2,3)) &amp; IF(ISBLANK(stand_md!AX4),"","_") &amp; UPPER(LEFT(stand_md!AX4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AX$3,1) &amp; RIGHT(plant_md!AX$3,LEN(plant_md!AX$3)-FIND(" ",plant_md!AX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AX$1,"")</f>
         <v/>
       </c>
       <c r="AY25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AY$3,1) &amp; RIGHT(plant_md!AY$3,LEN(plant_md!AY$3)-FIND(" ",plant_md!AY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AY$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AY2),"","_") &amp; UPPER(LEFT(stand_md!AY2,3)) &amp; IF(ISBLANK(stand_md!AY4),"","_") &amp; UPPER(LEFT(stand_md!AY4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AY$3,1) &amp; RIGHT(plant_md!AY$3,LEN(plant_md!AY$3)-FIND(" ",plant_md!AY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AY$1,"")</f>
         <v/>
       </c>
       <c r="AZ25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AZ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AZ$3,1) &amp; RIGHT(plant_md!AZ$3,LEN(plant_md!AZ$3)-FIND(" ",plant_md!AZ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AZ$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AZ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AZ2),"","_") &amp; UPPER(LEFT(stand_md!AZ2,3)) &amp; IF(ISBLANK(stand_md!AZ4),"","_") &amp; UPPER(LEFT(stand_md!AZ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AZ$3,1) &amp; RIGHT(plant_md!AZ$3,LEN(plant_md!AZ$3)-FIND(" ",plant_md!AZ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AZ$1,"")</f>
         <v/>
       </c>
       <c r="BA25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BA$3,1) &amp; RIGHT(plant_md!BA$3,LEN(plant_md!BA$3)-FIND(" ",plant_md!BA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BA$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BA2),"","_") &amp; UPPER(LEFT(stand_md!BA2,3)) &amp; IF(ISBLANK(stand_md!BA4),"","_") &amp; UPPER(LEFT(stand_md!BA4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BA$3,1) &amp; RIGHT(plant_md!BA$3,LEN(plant_md!BA$3)-FIND(" ",plant_md!BA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BA$1,"")</f>
         <v/>
       </c>
       <c r="BB25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BB$3,1) &amp; RIGHT(plant_md!BB$3,LEN(plant_md!BB$3)-FIND(" ",plant_md!BB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BB$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BB2),"","_") &amp; UPPER(LEFT(stand_md!BB2,3)) &amp; IF(ISBLANK(stand_md!BB4),"","_") &amp; UPPER(LEFT(stand_md!BB4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BB$3,1) &amp; RIGHT(plant_md!BB$3,LEN(plant_md!BB$3)-FIND(" ",plant_md!BB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BB$1,"")</f>
         <v/>
       </c>
       <c r="BC25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BC$3,1) &amp; RIGHT(plant_md!BC$3,LEN(plant_md!BC$3)-FIND(" ",plant_md!BC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BC$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BC2),"","_") &amp; UPPER(LEFT(stand_md!BC2,3)) &amp; IF(ISBLANK(stand_md!BC4),"","_") &amp; UPPER(LEFT(stand_md!BC4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BC$3,1) &amp; RIGHT(plant_md!BC$3,LEN(plant_md!BC$3)-FIND(" ",plant_md!BC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BC$1,"")</f>
         <v/>
       </c>
       <c r="BD25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BD$3,1) &amp; RIGHT(plant_md!BD$3,LEN(plant_md!BD$3)-FIND(" ",plant_md!BD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BD$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BD2),"","_") &amp; UPPER(LEFT(stand_md!BD2,3)) &amp; IF(ISBLANK(stand_md!BD4),"","_") &amp; UPPER(LEFT(stand_md!BD4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BD$3,1) &amp; RIGHT(plant_md!BD$3,LEN(plant_md!BD$3)-FIND(" ",plant_md!BD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BD$1,"")</f>
         <v/>
       </c>
       <c r="BE25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BE$3,1) &amp; RIGHT(plant_md!BE$3,LEN(plant_md!BE$3)-FIND(" ",plant_md!BE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BE$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BE2),"","_") &amp; UPPER(LEFT(stand_md!BE2,3)) &amp; IF(ISBLANK(stand_md!BE4),"","_") &amp; UPPER(LEFT(stand_md!BE4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BE$3,1) &amp; RIGHT(plant_md!BE$3,LEN(plant_md!BE$3)-FIND(" ",plant_md!BE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BE$1,"")</f>
         <v/>
       </c>
       <c r="BF25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BF$3,1) &amp; RIGHT(plant_md!BF$3,LEN(plant_md!BF$3)-FIND(" ",plant_md!BF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BF$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BF2),"","_") &amp; UPPER(LEFT(stand_md!BF2,3)) &amp; IF(ISBLANK(stand_md!BF4),"","_") &amp; UPPER(LEFT(stand_md!BF4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BF$3,1) &amp; RIGHT(plant_md!BF$3,LEN(plant_md!BF$3)-FIND(" ",plant_md!BF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BF$1,"")</f>
         <v/>
       </c>
       <c r="BG25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BG$3,1) &amp; RIGHT(plant_md!BG$3,LEN(plant_md!BG$3)-FIND(" ",plant_md!BG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BG$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BG2),"","_") &amp; UPPER(LEFT(stand_md!BG2,3)) &amp; IF(ISBLANK(stand_md!BG4),"","_") &amp; UPPER(LEFT(stand_md!BG4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BG$3,1) &amp; RIGHT(plant_md!BG$3,LEN(plant_md!BG$3)-FIND(" ",plant_md!BG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BG$1,"")</f>
         <v/>
       </c>
       <c r="BH25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BH$3,1) &amp; RIGHT(plant_md!BH$3,LEN(plant_md!BH$3)-FIND(" ",plant_md!BH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BH$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BH2),"","_") &amp; UPPER(LEFT(stand_md!BH2,3)) &amp; IF(ISBLANK(stand_md!BH4),"","_") &amp; UPPER(LEFT(stand_md!BH4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BH$3,1) &amp; RIGHT(plant_md!BH$3,LEN(plant_md!BH$3)-FIND(" ",plant_md!BH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BH$1,"")</f>
         <v/>
       </c>
       <c r="BI25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BI$3,1) &amp; RIGHT(plant_md!BI$3,LEN(plant_md!BI$3)-FIND(" ",plant_md!BI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BI$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BI2),"","_") &amp; UPPER(LEFT(stand_md!BI2,3)) &amp; IF(ISBLANK(stand_md!BI4),"","_") &amp; UPPER(LEFT(stand_md!BI4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BI$3,1) &amp; RIGHT(plant_md!BI$3,LEN(plant_md!BI$3)-FIND(" ",plant_md!BI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BI$1,"")</f>
         <v/>
       </c>
       <c r="BJ25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BJ$3,1) &amp; RIGHT(plant_md!BJ$3,LEN(plant_md!BJ$3)-FIND(" ",plant_md!BJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BJ$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BJ2),"","_") &amp; UPPER(LEFT(stand_md!BJ2,3)) &amp; IF(ISBLANK(stand_md!BJ4),"","_") &amp; UPPER(LEFT(stand_md!BJ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BJ$3,1) &amp; RIGHT(plant_md!BJ$3,LEN(plant_md!BJ$3)-FIND(" ",plant_md!BJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BJ$1,"")</f>
         <v/>
       </c>
       <c r="BK25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BK$3,1) &amp; RIGHT(plant_md!BK$3,LEN(plant_md!BK$3)-FIND(" ",plant_md!BK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BK$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BK2),"","_") &amp; UPPER(LEFT(stand_md!BK2,3)) &amp; IF(ISBLANK(stand_md!BK4),"","_") &amp; UPPER(LEFT(stand_md!BK4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BK$3,1) &amp; RIGHT(plant_md!BK$3,LEN(plant_md!BK$3)-FIND(" ",plant_md!BK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BK$1,"")</f>
         <v/>
       </c>
       <c r="BL25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BL$3,1) &amp; RIGHT(plant_md!BL$3,LEN(plant_md!BL$3)-FIND(" ",plant_md!BL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BL$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BL2),"","_") &amp; UPPER(LEFT(stand_md!BL2,3)) &amp; IF(ISBLANK(stand_md!BL4),"","_") &amp; UPPER(LEFT(stand_md!BL4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BL$3,1) &amp; RIGHT(plant_md!BL$3,LEN(plant_md!BL$3)-FIND(" ",plant_md!BL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BL$1,"")</f>
         <v/>
       </c>
       <c r="BM25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BM$3,1) &amp; RIGHT(plant_md!BM$3,LEN(plant_md!BM$3)-FIND(" ",plant_md!BM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BM$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BM2),"","_") &amp; UPPER(LEFT(stand_md!BM2,3)) &amp; IF(ISBLANK(stand_md!BM4),"","_") &amp; UPPER(LEFT(stand_md!BM4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BM$3,1) &amp; RIGHT(plant_md!BM$3,LEN(plant_md!BM$3)-FIND(" ",plant_md!BM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BM$1,"")</f>
         <v/>
       </c>
       <c r="BN25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BN$3,1) &amp; RIGHT(plant_md!BN$3,LEN(plant_md!BN$3)-FIND(" ",plant_md!BN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BN$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BN2),"","_") &amp; UPPER(LEFT(stand_md!BN2,3)) &amp; IF(ISBLANK(stand_md!BN4),"","_") &amp; UPPER(LEFT(stand_md!BN4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BN$3,1) &amp; RIGHT(plant_md!BN$3,LEN(plant_md!BN$3)-FIND(" ",plant_md!BN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BN$1,"")</f>
         <v/>
       </c>
       <c r="BO25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BO$3,1) &amp; RIGHT(plant_md!BO$3,LEN(plant_md!BO$3)-FIND(" ",plant_md!BO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BO$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BO2),"","_") &amp; UPPER(LEFT(stand_md!BO2,3)) &amp; IF(ISBLANK(stand_md!BO4),"","_") &amp; UPPER(LEFT(stand_md!BO4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BO$3,1) &amp; RIGHT(plant_md!BO$3,LEN(plant_md!BO$3)-FIND(" ",plant_md!BO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BO$1,"")</f>
         <v/>
       </c>
       <c r="BP25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BP$3,1) &amp; RIGHT(plant_md!BP$3,LEN(plant_md!BP$3)-FIND(" ",plant_md!BP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BP$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BP2),"","_") &amp; UPPER(LEFT(stand_md!BP2,3)) &amp; IF(ISBLANK(stand_md!BP4),"","_") &amp; UPPER(LEFT(stand_md!BP4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BP$3,1) &amp; RIGHT(plant_md!BP$3,LEN(plant_md!BP$3)-FIND(" ",plant_md!BP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BP$1,"")</f>
         <v/>
       </c>
       <c r="BQ25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BQ$3,1) &amp; RIGHT(plant_md!BQ$3,LEN(plant_md!BQ$3)-FIND(" ",plant_md!BQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BQ$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BQ2),"","_") &amp; UPPER(LEFT(stand_md!BQ2,3)) &amp; IF(ISBLANK(stand_md!BQ4),"","_") &amp; UPPER(LEFT(stand_md!BQ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BQ$3,1) &amp; RIGHT(plant_md!BQ$3,LEN(plant_md!BQ$3)-FIND(" ",plant_md!BQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BQ$1,"")</f>
         <v/>
       </c>
       <c r="BR25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BR$3,1) &amp; RIGHT(plant_md!BR$3,LEN(plant_md!BR$3)-FIND(" ",plant_md!BR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BR$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BR2),"","_") &amp; UPPER(LEFT(stand_md!BR2,3)) &amp; IF(ISBLANK(stand_md!BR4),"","_") &amp; UPPER(LEFT(stand_md!BR4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BR$3,1) &amp; RIGHT(plant_md!BR$3,LEN(plant_md!BR$3)-FIND(" ",plant_md!BR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BR$1,"")</f>
         <v/>
       </c>
       <c r="BS25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BS$3,1) &amp; RIGHT(plant_md!BS$3,LEN(plant_md!BS$3)-FIND(" ",plant_md!BS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BS$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BS2),"","_") &amp; UPPER(LEFT(stand_md!BS2,3)) &amp; IF(ISBLANK(stand_md!BS4),"","_") &amp; UPPER(LEFT(stand_md!BS4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BS$3,1) &amp; RIGHT(plant_md!BS$3,LEN(plant_md!BS$3)-FIND(" ",plant_md!BS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BS$1,"")</f>
         <v/>
       </c>
       <c r="BT25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BT$3,1) &amp; RIGHT(plant_md!BT$3,LEN(plant_md!BT$3)-FIND(" ",plant_md!BT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BT$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BT2),"","_") &amp; UPPER(LEFT(stand_md!BT2,3)) &amp; IF(ISBLANK(stand_md!BT4),"","_") &amp; UPPER(LEFT(stand_md!BT4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BT$3,1) &amp; RIGHT(plant_md!BT$3,LEN(plant_md!BT$3)-FIND(" ",plant_md!BT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BT$1,"")</f>
         <v/>
       </c>
       <c r="BU25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BU$3,1) &amp; RIGHT(plant_md!BU$3,LEN(plant_md!BU$3)-FIND(" ",plant_md!BU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BU$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BU2),"","_") &amp; UPPER(LEFT(stand_md!BU2,3)) &amp; IF(ISBLANK(stand_md!BU4),"","_") &amp; UPPER(LEFT(stand_md!BU4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BU$3,1) &amp; RIGHT(plant_md!BU$3,LEN(plant_md!BU$3)-FIND(" ",plant_md!BU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BU$1,"")</f>
         <v/>
       </c>
       <c r="BV25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BV$3,1) &amp; RIGHT(plant_md!BV$3,LEN(plant_md!BV$3)-FIND(" ",plant_md!BV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BV$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BV2),"","_") &amp; UPPER(LEFT(stand_md!BV2,3)) &amp; IF(ISBLANK(stand_md!BV4),"","_") &amp; UPPER(LEFT(stand_md!BV4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BV$3,1) &amp; RIGHT(plant_md!BV$3,LEN(plant_md!BV$3)-FIND(" ",plant_md!BV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BV$1,"")</f>
         <v/>
       </c>
       <c r="BW25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BW$3,1) &amp; RIGHT(plant_md!BW$3,LEN(plant_md!BW$3)-FIND(" ",plant_md!BW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BW$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BW2),"","_") &amp; UPPER(LEFT(stand_md!BW2,3)) &amp; IF(ISBLANK(stand_md!BW4),"","_") &amp; UPPER(LEFT(stand_md!BW4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BW$3,1) &amp; RIGHT(plant_md!BW$3,LEN(plant_md!BW$3)-FIND(" ",plant_md!BW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BW$1,"")</f>
         <v/>
       </c>
       <c r="BX25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BX$3,1) &amp; RIGHT(plant_md!BX$3,LEN(plant_md!BX$3)-FIND(" ",plant_md!BX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BX$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BX2),"","_") &amp; UPPER(LEFT(stand_md!BX2,3)) &amp; IF(ISBLANK(stand_md!BX4),"","_") &amp; UPPER(LEFT(stand_md!BX4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BX$3,1) &amp; RIGHT(plant_md!BX$3,LEN(plant_md!BX$3)-FIND(" ",plant_md!BX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BX$1,"")</f>
         <v/>
       </c>
       <c r="BY25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BY$3,1) &amp; RIGHT(plant_md!BY$3,LEN(plant_md!BY$3)-FIND(" ",plant_md!BY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BY$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BY2),"","_") &amp; UPPER(LEFT(stand_md!BY2,3)) &amp; IF(ISBLANK(stand_md!BY4),"","_") &amp; UPPER(LEFT(stand_md!BY4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BY$3,1) &amp; RIGHT(plant_md!BY$3,LEN(plant_md!BY$3)-FIND(" ",plant_md!BY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BY$1,"")</f>
         <v/>
       </c>
       <c r="BZ25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BZ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BZ$3,1) &amp; RIGHT(plant_md!BZ$3,LEN(plant_md!BZ$3)-FIND(" ",plant_md!BZ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BZ$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BZ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BZ2),"","_") &amp; UPPER(LEFT(stand_md!BZ2,3)) &amp; IF(ISBLANK(stand_md!BZ4),"","_") &amp; UPPER(LEFT(stand_md!BZ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BZ$3,1) &amp; RIGHT(plant_md!BZ$3,LEN(plant_md!BZ$3)-FIND(" ",plant_md!BZ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BZ$1,"")</f>
         <v/>
       </c>
       <c r="CA25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CA$3,1) &amp; RIGHT(plant_md!CA$3,LEN(plant_md!CA$3)-FIND(" ",plant_md!CA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CA$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CA2),"","_") &amp; UPPER(LEFT(stand_md!CA2,3)) &amp; IF(ISBLANK(stand_md!CA4),"","_") &amp; UPPER(LEFT(stand_md!CA4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CA$3,1) &amp; RIGHT(plant_md!CA$3,LEN(plant_md!CA$3)-FIND(" ",plant_md!CA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CA$1,"")</f>
         <v/>
       </c>
       <c r="CB25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CB$3,1) &amp; RIGHT(plant_md!CB$3,LEN(plant_md!CB$3)-FIND(" ",plant_md!CB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CB$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CB2),"","_") &amp; UPPER(LEFT(stand_md!CB2,3)) &amp; IF(ISBLANK(stand_md!CB4),"","_") &amp; UPPER(LEFT(stand_md!CB4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CB$3,1) &amp; RIGHT(plant_md!CB$3,LEN(plant_md!CB$3)-FIND(" ",plant_md!CB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CB$1,"")</f>
         <v/>
       </c>
       <c r="CC25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CC$3,1) &amp; RIGHT(plant_md!CC$3,LEN(plant_md!CC$3)-FIND(" ",plant_md!CC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CC$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CC2),"","_") &amp; UPPER(LEFT(stand_md!CC2,3)) &amp; IF(ISBLANK(stand_md!CC4),"","_") &amp; UPPER(LEFT(stand_md!CC4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CC$3,1) &amp; RIGHT(plant_md!CC$3,LEN(plant_md!CC$3)-FIND(" ",plant_md!CC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CC$1,"")</f>
         <v/>
       </c>
       <c r="CD25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CD$3,1) &amp; RIGHT(plant_md!CD$3,LEN(plant_md!CD$3)-FIND(" ",plant_md!CD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CD$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CD2),"","_") &amp; UPPER(LEFT(stand_md!CD2,3)) &amp; IF(ISBLANK(stand_md!CD4),"","_") &amp; UPPER(LEFT(stand_md!CD4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CD$3,1) &amp; RIGHT(plant_md!CD$3,LEN(plant_md!CD$3)-FIND(" ",plant_md!CD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CD$1,"")</f>
         <v/>
       </c>
       <c r="CE25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CE$3,1) &amp; RIGHT(plant_md!CE$3,LEN(plant_md!CE$3)-FIND(" ",plant_md!CE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CE$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CE2),"","_") &amp; UPPER(LEFT(stand_md!CE2,3)) &amp; IF(ISBLANK(stand_md!CE4),"","_") &amp; UPPER(LEFT(stand_md!CE4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CE$3,1) &amp; RIGHT(plant_md!CE$3,LEN(plant_md!CE$3)-FIND(" ",plant_md!CE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CE$1,"")</f>
         <v/>
       </c>
       <c r="CF25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CF$3,1) &amp; RIGHT(plant_md!CF$3,LEN(plant_md!CF$3)-FIND(" ",plant_md!CF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CF$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CF2),"","_") &amp; UPPER(LEFT(stand_md!CF2,3)) &amp; IF(ISBLANK(stand_md!CF4),"","_") &amp; UPPER(LEFT(stand_md!CF4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CF$3,1) &amp; RIGHT(plant_md!CF$3,LEN(plant_md!CF$3)-FIND(" ",plant_md!CF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CF$1,"")</f>
         <v/>
       </c>
       <c r="CG25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CG$3,1) &amp; RIGHT(plant_md!CG$3,LEN(plant_md!CG$3)-FIND(" ",plant_md!CG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CG$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CG2),"","_") &amp; UPPER(LEFT(stand_md!CG2,3)) &amp; IF(ISBLANK(stand_md!CG4),"","_") &amp; UPPER(LEFT(stand_md!CG4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CG$3,1) &amp; RIGHT(plant_md!CG$3,LEN(plant_md!CG$3)-FIND(" ",plant_md!CG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CG$1,"")</f>
         <v/>
       </c>
       <c r="CH25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CH$3,1) &amp; RIGHT(plant_md!CH$3,LEN(plant_md!CH$3)-FIND(" ",plant_md!CH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CH$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CH2),"","_") &amp; UPPER(LEFT(stand_md!CH2,3)) &amp; IF(ISBLANK(stand_md!CH4),"","_") &amp; UPPER(LEFT(stand_md!CH4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CH$3,1) &amp; RIGHT(plant_md!CH$3,LEN(plant_md!CH$3)-FIND(" ",plant_md!CH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CH$1,"")</f>
         <v/>
       </c>
       <c r="CI25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CI$3,1) &amp; RIGHT(plant_md!CI$3,LEN(plant_md!CI$3)-FIND(" ",plant_md!CI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CI$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CI2),"","_") &amp; UPPER(LEFT(stand_md!CI2,3)) &amp; IF(ISBLANK(stand_md!CI4),"","_") &amp; UPPER(LEFT(stand_md!CI4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CI$3,1) &amp; RIGHT(plant_md!CI$3,LEN(plant_md!CI$3)-FIND(" ",plant_md!CI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CI$1,"")</f>
         <v/>
       </c>
       <c r="CJ25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CJ$3,1) &amp; RIGHT(plant_md!CJ$3,LEN(plant_md!CJ$3)-FIND(" ",plant_md!CJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CJ$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CJ2),"","_") &amp; UPPER(LEFT(stand_md!CJ2,3)) &amp; IF(ISBLANK(stand_md!CJ4),"","_") &amp; UPPER(LEFT(stand_md!CJ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CJ$3,1) &amp; RIGHT(plant_md!CJ$3,LEN(plant_md!CJ$3)-FIND(" ",plant_md!CJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CJ$1,"")</f>
         <v/>
       </c>
       <c r="CK25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CK$3,1) &amp; RIGHT(plant_md!CK$3,LEN(plant_md!CK$3)-FIND(" ",plant_md!CK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CK$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CK2),"","_") &amp; UPPER(LEFT(stand_md!CK2,3)) &amp; IF(ISBLANK(stand_md!CK4),"","_") &amp; UPPER(LEFT(stand_md!CK4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CK$3,1) &amp; RIGHT(plant_md!CK$3,LEN(plant_md!CK$3)-FIND(" ",plant_md!CK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CK$1,"")</f>
         <v/>
       </c>
       <c r="CL25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CL$3,1) &amp; RIGHT(plant_md!CL$3,LEN(plant_md!CL$3)-FIND(" ",plant_md!CL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CL$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CL2),"","_") &amp; UPPER(LEFT(stand_md!CL2,3)) &amp; IF(ISBLANK(stand_md!CL4),"","_") &amp; UPPER(LEFT(stand_md!CL4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CL$3,1) &amp; RIGHT(plant_md!CL$3,LEN(plant_md!CL$3)-FIND(" ",plant_md!CL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CL$1,"")</f>
         <v/>
       </c>
       <c r="CM25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CM$3,1) &amp; RIGHT(plant_md!CM$3,LEN(plant_md!CM$3)-FIND(" ",plant_md!CM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CM$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CM2),"","_") &amp; UPPER(LEFT(stand_md!CM2,3)) &amp; IF(ISBLANK(stand_md!CM4),"","_") &amp; UPPER(LEFT(stand_md!CM4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CM$3,1) &amp; RIGHT(plant_md!CM$3,LEN(plant_md!CM$3)-FIND(" ",plant_md!CM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CM$1,"")</f>
         <v/>
       </c>
       <c r="CN25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CN$3,1) &amp; RIGHT(plant_md!CN$3,LEN(plant_md!CN$3)-FIND(" ",plant_md!CN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CN$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CN2),"","_") &amp; UPPER(LEFT(stand_md!CN2,3)) &amp; IF(ISBLANK(stand_md!CN4),"","_") &amp; UPPER(LEFT(stand_md!CN4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CN$3,1) &amp; RIGHT(plant_md!CN$3,LEN(plant_md!CN$3)-FIND(" ",plant_md!CN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CN$1,"")</f>
         <v/>
       </c>
       <c r="CO25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CO$3,1) &amp; RIGHT(plant_md!CO$3,LEN(plant_md!CO$3)-FIND(" ",plant_md!CO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CO$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CO2),"","_") &amp; UPPER(LEFT(stand_md!CO2,3)) &amp; IF(ISBLANK(stand_md!CO4),"","_") &amp; UPPER(LEFT(stand_md!CO4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CO$3,1) &amp; RIGHT(plant_md!CO$3,LEN(plant_md!CO$3)-FIND(" ",plant_md!CO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CO$1,"")</f>
         <v/>
       </c>
       <c r="CP25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CP$3,1) &amp; RIGHT(plant_md!CP$3,LEN(plant_md!CP$3)-FIND(" ",plant_md!CP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CP$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CP2),"","_") &amp; UPPER(LEFT(stand_md!CP2,3)) &amp; IF(ISBLANK(stand_md!CP4),"","_") &amp; UPPER(LEFT(stand_md!CP4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CP$3,1) &amp; RIGHT(plant_md!CP$3,LEN(plant_md!CP$3)-FIND(" ",plant_md!CP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CP$1,"")</f>
         <v/>
       </c>
       <c r="CQ25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CQ$3,1) &amp; RIGHT(plant_md!CQ$3,LEN(plant_md!CQ$3)-FIND(" ",plant_md!CQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CQ$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CQ2),"","_") &amp; UPPER(LEFT(stand_md!CQ2,3)) &amp; IF(ISBLANK(stand_md!CQ4),"","_") &amp; UPPER(LEFT(stand_md!CQ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CQ$3,1) &amp; RIGHT(plant_md!CQ$3,LEN(plant_md!CQ$3)-FIND(" ",plant_md!CQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CQ$1,"")</f>
         <v/>
       </c>
       <c r="CR25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CR$3,1) &amp; RIGHT(plant_md!CR$3,LEN(plant_md!CR$3)-FIND(" ",plant_md!CR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CR$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CR2),"","_") &amp; UPPER(LEFT(stand_md!CR2,3)) &amp; IF(ISBLANK(stand_md!CR4),"","_") &amp; UPPER(LEFT(stand_md!CR4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CR$3,1) &amp; RIGHT(plant_md!CR$3,LEN(plant_md!CR$3)-FIND(" ",plant_md!CR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CR$1,"")</f>
         <v/>
       </c>
       <c r="CS25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CS$3,1) &amp; RIGHT(plant_md!CS$3,LEN(plant_md!CS$3)-FIND(" ",plant_md!CS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CS$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CS2),"","_") &amp; UPPER(LEFT(stand_md!CS2,3)) &amp; IF(ISBLANK(stand_md!CS4),"","_") &amp; UPPER(LEFT(stand_md!CS4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CS$3,1) &amp; RIGHT(plant_md!CS$3,LEN(plant_md!CS$3)-FIND(" ",plant_md!CS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CS$1,"")</f>
         <v/>
       </c>
       <c r="CT25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CT$3,1) &amp; RIGHT(plant_md!CT$3,LEN(plant_md!CT$3)-FIND(" ",plant_md!CT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CT$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CT2),"","_") &amp; UPPER(LEFT(stand_md!CT2,3)) &amp; IF(ISBLANK(stand_md!CT4),"","_") &amp; UPPER(LEFT(stand_md!CT4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CT$3,1) &amp; RIGHT(plant_md!CT$3,LEN(plant_md!CT$3)-FIND(" ",plant_md!CT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CT$1,"")</f>
         <v/>
       </c>
       <c r="CU25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CU$3,1) &amp; RIGHT(plant_md!CU$3,LEN(plant_md!CU$3)-FIND(" ",plant_md!CU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CU$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CU2),"","_") &amp; UPPER(LEFT(stand_md!CU2,3)) &amp; IF(ISBLANK(stand_md!CU4),"","_") &amp; UPPER(LEFT(stand_md!CU4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CU$3,1) &amp; RIGHT(plant_md!CU$3,LEN(plant_md!CU$3)-FIND(" ",plant_md!CU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CU$1,"")</f>
         <v/>
       </c>
       <c r="CV25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CV$3,1) &amp; RIGHT(plant_md!CV$3,LEN(plant_md!CV$3)-FIND(" ",plant_md!CV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CV$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CV2),"","_") &amp; UPPER(LEFT(stand_md!CV2,3)) &amp; IF(ISBLANK(stand_md!CV4),"","_") &amp; UPPER(LEFT(stand_md!CV4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CV$3,1) &amp; RIGHT(plant_md!CV$3,LEN(plant_md!CV$3)-FIND(" ",plant_md!CV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CV$1,"")</f>
         <v/>
       </c>
       <c r="CW25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CW$3,1) &amp; RIGHT(plant_md!CW$3,LEN(plant_md!CW$3)-FIND(" ",plant_md!CW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CW$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CW2),"","_") &amp; UPPER(LEFT(stand_md!CW2,3)) &amp; IF(ISBLANK(stand_md!CW4),"","_") &amp; UPPER(LEFT(stand_md!CW4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CW$3,1) &amp; RIGHT(plant_md!CW$3,LEN(plant_md!CW$3)-FIND(" ",plant_md!CW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CW$1,"")</f>
         <v/>
       </c>
       <c r="CX25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CX$3,1) &amp; RIGHT(plant_md!CX$3,LEN(plant_md!CX$3)-FIND(" ",plant_md!CX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CX$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CX2),"","_") &amp; UPPER(LEFT(stand_md!CX2,3)) &amp; IF(ISBLANK(stand_md!CX4),"","_") &amp; UPPER(LEFT(stand_md!CX4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CX$3,1) &amp; RIGHT(plant_md!CX$3,LEN(plant_md!CX$3)-FIND(" ",plant_md!CX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CX$1,"")</f>
         <v/>
       </c>
       <c r="CY25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; "_" &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CY$3,1) &amp; RIGHT(plant_md!CY$3,LEN(plant_md!CY$3)-FIND(" ",plant_md!CY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CY$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CY2),"","_") &amp; UPPER(LEFT(stand_md!CY2,3)) &amp; IF(ISBLANK(stand_md!CY4),"","_") &amp; UPPER(LEFT(stand_md!CY4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CY$3,1) &amp; RIGHT(plant_md!CY$3,LEN(plant_md!CY$3)-FIND(" ",plant_md!CY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CY$1,"")</f>
         <v/>
       </c>
     </row>
@@ -10950,7 +10946,6 @@
       <c r="C37" s="125"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="8">
     <mergeCell ref="F27:F31"/>
     <mergeCell ref="E27:E31"/>
@@ -10961,7 +10956,7 @@
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="B28:B31"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="24">
+  <dataValidations count="24">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Plant code" prompt="Unique code for each measured plant in the stand, as given by contributor." sqref="D2:CY2"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Scientific name" prompt="Species name without author abbreviation (e.g. Pinus pinaster)" sqref="D3:CY3"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Remarks" prompt="Please add any information relevant to plant-specific peculiarities that may not have been adequately captured by the plant-level metadata." sqref="D24:CY24"/>

</xml_diff>

<commit_message>
fixed stand cells corrected in plant names
</commit_message>
<xml_diff>
--- a/sfnform/static/sfnform/media/sapfluxnet_metadata_template.xlsx
+++ b/sfnform/static/sfnform/media/sapfluxnet_metadata_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10470" windowHeight="8085" tabRatio="796"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="14415" windowHeight="11040" tabRatio="796" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="site_md" sheetId="1" r:id="rId1"/>
@@ -5259,7 +5259,7 @@
   </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.7109375" defaultRowHeight="12.75"/>
   <cols>
@@ -10471,403 +10471,403 @@
         <v>1037</v>
       </c>
       <c r="D25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!D$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!D2),"","_") &amp; UPPER(LEFT(stand_md!D2,3)) &amp; IF(ISBLANK(stand_md!D4),"","_") &amp; UPPER(LEFT(stand_md!D4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!D$3,1) &amp; RIGHT(plant_md!D$3,LEN(plant_md!D$3)-FIND(" ",plant_md!D$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!B3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!B3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!D$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!D$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!D$3,1) &amp; RIGHT(plant_md!D$3,LEN(plant_md!D$3)-FIND(" ",plant_md!D$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!B3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!B3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!D$1,"")</f>
         <v/>
       </c>
       <c r="E25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!E$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!E2),"","_") &amp; UPPER(LEFT(stand_md!E2,3)) &amp; IF(ISBLANK(stand_md!E4),"","_") &amp; UPPER(LEFT(stand_md!E4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!E$3,1) &amp; RIGHT(plant_md!E$3,LEN(plant_md!E$3)-FIND(" ",plant_md!E$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!C3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!C3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!E$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!E$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!E$3,1) &amp; RIGHT(plant_md!E$3,LEN(plant_md!E$3)-FIND(" ",plant_md!E$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!C3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!C3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!E$1,"")</f>
         <v/>
       </c>
       <c r="F25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!F$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!F2),"","_") &amp; UPPER(LEFT(stand_md!F2,3)) &amp; IF(ISBLANK(stand_md!F4),"","_") &amp; UPPER(LEFT(stand_md!F4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!F$3,1) &amp; RIGHT(plant_md!F$3,LEN(plant_md!F$3)-FIND(" ",plant_md!F$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!D3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!D3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!F$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!F$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!F$3,1) &amp; RIGHT(plant_md!F$3,LEN(plant_md!F$3)-FIND(" ",plant_md!F$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!D3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!D3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!F$1,"")</f>
         <v/>
       </c>
       <c r="G25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!G$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!G2),"","_") &amp; UPPER(LEFT(stand_md!G2,3)) &amp; IF(ISBLANK(stand_md!G4),"","_") &amp; UPPER(LEFT(stand_md!G4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!G$3,1) &amp; RIGHT(plant_md!G$3,LEN(plant_md!G$3)-FIND(" ",plant_md!G$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!E3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!E3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!G$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!G$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!G$3,1) &amp; RIGHT(plant_md!G$3,LEN(plant_md!G$3)-FIND(" ",plant_md!G$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!E3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!E3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!G$1,"")</f>
         <v/>
       </c>
       <c r="H25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!H$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!H2),"","_") &amp; UPPER(LEFT(stand_md!H2,3)) &amp; IF(ISBLANK(stand_md!H4),"","_") &amp; UPPER(LEFT(stand_md!H4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!H$3,1) &amp; RIGHT(plant_md!H$3,LEN(plant_md!H$3)-FIND(" ",plant_md!H$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!F3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!F3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!H$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!H$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!H$3,1) &amp; RIGHT(plant_md!H$3,LEN(plant_md!H$3)-FIND(" ",plant_md!H$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!F3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!F3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!H$1,"")</f>
         <v/>
       </c>
       <c r="I25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!I$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!I2),"","_") &amp; UPPER(LEFT(stand_md!I2,3)) &amp; IF(ISBLANK(stand_md!I4),"","_") &amp; UPPER(LEFT(stand_md!I4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!I$3,1) &amp; RIGHT(plant_md!I$3,LEN(plant_md!I$3)-FIND(" ",plant_md!I$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!G3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!G3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!I$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!I$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!I$3,1) &amp; RIGHT(plant_md!I$3,LEN(plant_md!I$3)-FIND(" ",plant_md!I$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!G3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!G3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!I$1,"")</f>
         <v/>
       </c>
       <c r="J25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!J$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!J2),"","_") &amp; UPPER(LEFT(stand_md!J2,3)) &amp; IF(ISBLANK(stand_md!J4),"","_") &amp; UPPER(LEFT(stand_md!J4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!J$3,1) &amp; RIGHT(plant_md!J$3,LEN(plant_md!J$3)-FIND(" ",plant_md!J$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!H3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!H3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!J$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!J$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!J$3,1) &amp; RIGHT(plant_md!J$3,LEN(plant_md!J$3)-FIND(" ",plant_md!J$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!H3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!H3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!J$1,"")</f>
         <v/>
       </c>
       <c r="K25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!K$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!K2),"","_") &amp; UPPER(LEFT(stand_md!K2,3)) &amp; IF(ISBLANK(stand_md!K4),"","_") &amp; UPPER(LEFT(stand_md!K4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!K$3,1) &amp; RIGHT(plant_md!K$3,LEN(plant_md!K$3)-FIND(" ",plant_md!K$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!I3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!I3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!K$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!K$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!K$3,1) &amp; RIGHT(plant_md!K$3,LEN(plant_md!K$3)-FIND(" ",plant_md!K$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!I3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!I3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!K$1,"")</f>
         <v/>
       </c>
       <c r="L25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!L$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!L2),"","_") &amp; UPPER(LEFT(stand_md!L2,3)) &amp; IF(ISBLANK(stand_md!L4),"","_") &amp; UPPER(LEFT(stand_md!L4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!L$3,1) &amp; RIGHT(plant_md!L$3,LEN(plant_md!L$3)-FIND(" ",plant_md!L$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!J3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!J3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!L$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!L$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!L$3,1) &amp; RIGHT(plant_md!L$3,LEN(plant_md!L$3)-FIND(" ",plant_md!L$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!J3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!J3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!L$1,"")</f>
         <v/>
       </c>
       <c r="M25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!M$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!M2),"","_") &amp; UPPER(LEFT(stand_md!M2,3)) &amp; IF(ISBLANK(stand_md!M4),"","_") &amp; UPPER(LEFT(stand_md!M4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!M$3,1) &amp; RIGHT(plant_md!M$3,LEN(plant_md!M$3)-FIND(" ",plant_md!M$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!K3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!K3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!M$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!M$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!M$3,1) &amp; RIGHT(plant_md!M$3,LEN(plant_md!M$3)-FIND(" ",plant_md!M$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!K3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!K3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!M$1,"")</f>
         <v/>
       </c>
       <c r="N25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!N$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!N2),"","_") &amp; UPPER(LEFT(stand_md!N2,3)) &amp; IF(ISBLANK(stand_md!N4),"","_") &amp; UPPER(LEFT(stand_md!N4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!N$3,1) &amp; RIGHT(plant_md!N$3,LEN(plant_md!N$3)-FIND(" ",plant_md!N$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!L3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!L3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!N$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!N$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!N$3,1) &amp; RIGHT(plant_md!N$3,LEN(plant_md!N$3)-FIND(" ",plant_md!N$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!L3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!L3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!N$1,"")</f>
         <v/>
       </c>
       <c r="O25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!O$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!O2),"","_") &amp; UPPER(LEFT(stand_md!O2,3)) &amp; IF(ISBLANK(stand_md!O4),"","_") &amp; UPPER(LEFT(stand_md!O4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!O$3,1) &amp; RIGHT(plant_md!O$3,LEN(plant_md!O$3)-FIND(" ",plant_md!O$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!M3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!M3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!O$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!O$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!O$3,1) &amp; RIGHT(plant_md!O$3,LEN(plant_md!O$3)-FIND(" ",plant_md!O$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!M3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!M3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!O$1,"")</f>
         <v/>
       </c>
       <c r="P25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!P$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!P2),"","_") &amp; UPPER(LEFT(stand_md!P2,3)) &amp; IF(ISBLANK(stand_md!P4),"","_") &amp; UPPER(LEFT(stand_md!P4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!P$3,1) &amp; RIGHT(plant_md!P$3,LEN(plant_md!P$3)-FIND(" ",plant_md!P$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!N3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!N3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!P$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!P$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!P$3,1) &amp; RIGHT(plant_md!P$3,LEN(plant_md!P$3)-FIND(" ",plant_md!P$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!N3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!N3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!P$1,"")</f>
         <v/>
       </c>
       <c r="Q25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!Q$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!Q2),"","_") &amp; UPPER(LEFT(stand_md!Q2,3)) &amp; IF(ISBLANK(stand_md!Q4),"","_") &amp; UPPER(LEFT(stand_md!Q4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Q$3,1) &amp; RIGHT(plant_md!Q$3,LEN(plant_md!Q$3)-FIND(" ",plant_md!Q$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!O3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!O3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Q$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!Q$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Q$3,1) &amp; RIGHT(plant_md!Q$3,LEN(plant_md!Q$3)-FIND(" ",plant_md!Q$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!O3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!O3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Q$1,"")</f>
         <v/>
       </c>
       <c r="R25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!R$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!R2),"","_") &amp; UPPER(LEFT(stand_md!R2,3)) &amp; IF(ISBLANK(stand_md!R4),"","_") &amp; UPPER(LEFT(stand_md!R4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!R$3,1) &amp; RIGHT(plant_md!R$3,LEN(plant_md!R$3)-FIND(" ",plant_md!R$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!P3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!P3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!R$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!R$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!R$3,1) &amp; RIGHT(plant_md!R$3,LEN(plant_md!R$3)-FIND(" ",plant_md!R$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!P3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!P3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!R$1,"")</f>
         <v/>
       </c>
       <c r="S25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!S$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!S2),"","_") &amp; UPPER(LEFT(stand_md!S2,3)) &amp; IF(ISBLANK(stand_md!S4),"","_") &amp; UPPER(LEFT(stand_md!S4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!S$3,1) &amp; RIGHT(plant_md!S$3,LEN(plant_md!S$3)-FIND(" ",plant_md!S$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Q3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Q3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!S$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!S$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!S$3,1) &amp; RIGHT(plant_md!S$3,LEN(plant_md!S$3)-FIND(" ",plant_md!S$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Q3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Q3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!S$1,"")</f>
         <v/>
       </c>
       <c r="T25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!T$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!T2),"","_") &amp; UPPER(LEFT(stand_md!T2,3)) &amp; IF(ISBLANK(stand_md!T4),"","_") &amp; UPPER(LEFT(stand_md!T4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!T$3,1) &amp; RIGHT(plant_md!T$3,LEN(plant_md!T$3)-FIND(" ",plant_md!T$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!R3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!R3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!T$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!T$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!T$3,1) &amp; RIGHT(plant_md!T$3,LEN(plant_md!T$3)-FIND(" ",plant_md!T$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!R3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!R3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!T$1,"")</f>
         <v/>
       </c>
       <c r="U25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!U$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!U2),"","_") &amp; UPPER(LEFT(stand_md!U2,3)) &amp; IF(ISBLANK(stand_md!U4),"","_") &amp; UPPER(LEFT(stand_md!U4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!U$3,1) &amp; RIGHT(plant_md!U$3,LEN(plant_md!U$3)-FIND(" ",plant_md!U$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!S3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!S3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!U$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!U$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!U$3,1) &amp; RIGHT(plant_md!U$3,LEN(plant_md!U$3)-FIND(" ",plant_md!U$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!S3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!S3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!U$1,"")</f>
         <v/>
       </c>
       <c r="V25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!V$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!V2),"","_") &amp; UPPER(LEFT(stand_md!V2,3)) &amp; IF(ISBLANK(stand_md!V4),"","_") &amp; UPPER(LEFT(stand_md!V4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!V$3,1) &amp; RIGHT(plant_md!V$3,LEN(plant_md!V$3)-FIND(" ",plant_md!V$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!T3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!T3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!V$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!V$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!V$3,1) &amp; RIGHT(plant_md!V$3,LEN(plant_md!V$3)-FIND(" ",plant_md!V$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!T3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!T3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!V$1,"")</f>
         <v/>
       </c>
       <c r="W25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!W$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!W2),"","_") &amp; UPPER(LEFT(stand_md!W2,3)) &amp; IF(ISBLANK(stand_md!W4),"","_") &amp; UPPER(LEFT(stand_md!W4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!W$3,1) &amp; RIGHT(plant_md!W$3,LEN(plant_md!W$3)-FIND(" ",plant_md!W$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!U3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!U3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!W$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!W$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!W$3,1) &amp; RIGHT(plant_md!W$3,LEN(plant_md!W$3)-FIND(" ",plant_md!W$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!U3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!U3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!W$1,"")</f>
         <v/>
       </c>
       <c r="X25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!X$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!X2),"","_") &amp; UPPER(LEFT(stand_md!X2,3)) &amp; IF(ISBLANK(stand_md!X4),"","_") &amp; UPPER(LEFT(stand_md!X4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!X$3,1) &amp; RIGHT(plant_md!X$3,LEN(plant_md!X$3)-FIND(" ",plant_md!X$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!V3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!V3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!X$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!X$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!X$3,1) &amp; RIGHT(plant_md!X$3,LEN(plant_md!X$3)-FIND(" ",plant_md!X$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!V3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!V3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!X$1,"")</f>
         <v/>
       </c>
       <c r="Y25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!Y$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!Y2),"","_") &amp; UPPER(LEFT(stand_md!Y2,3)) &amp; IF(ISBLANK(stand_md!Y4),"","_") &amp; UPPER(LEFT(stand_md!Y4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Y$3,1) &amp; RIGHT(plant_md!Y$3,LEN(plant_md!Y$3)-FIND(" ",plant_md!Y$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!W3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!W3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Y$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!Y$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Y$3,1) &amp; RIGHT(plant_md!Y$3,LEN(plant_md!Y$3)-FIND(" ",plant_md!Y$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!W3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!W3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Y$1,"")</f>
         <v/>
       </c>
       <c r="Z25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!Z$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!Z2),"","_") &amp; UPPER(LEFT(stand_md!Z2,3)) &amp; IF(ISBLANK(stand_md!Z4),"","_") &amp; UPPER(LEFT(stand_md!Z4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Z$3,1) &amp; RIGHT(plant_md!Z$3,LEN(plant_md!Z$3)-FIND(" ",plant_md!Z$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!X3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!X3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Z$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!Z$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Z$3,1) &amp; RIGHT(plant_md!Z$3,LEN(plant_md!Z$3)-FIND(" ",plant_md!Z$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!X3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!X3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Z$1,"")</f>
         <v/>
       </c>
       <c r="AA25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AA2),"","_") &amp; UPPER(LEFT(stand_md!AA2,3)) &amp; IF(ISBLANK(stand_md!AA4),"","_") &amp; UPPER(LEFT(stand_md!AA4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AA$3,1) &amp; RIGHT(plant_md!AA$3,LEN(plant_md!AA$3)-FIND(" ",plant_md!AA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Y3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Y3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AA$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AA$3,1) &amp; RIGHT(plant_md!AA$3,LEN(plant_md!AA$3)-FIND(" ",plant_md!AA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Y3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Y3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AA$1,"")</f>
         <v/>
       </c>
       <c r="AB25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AB2),"","_") &amp; UPPER(LEFT(stand_md!AB2,3)) &amp; IF(ISBLANK(stand_md!AB4),"","_") &amp; UPPER(LEFT(stand_md!AB4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AB$3,1) &amp; RIGHT(plant_md!AB$3,LEN(plant_md!AB$3)-FIND(" ",plant_md!AB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Z3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Z3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AB$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AB$3,1) &amp; RIGHT(plant_md!AB$3,LEN(plant_md!AB$3)-FIND(" ",plant_md!AB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Z3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Z3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AB$1,"")</f>
         <v/>
       </c>
       <c r="AC25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AC2),"","_") &amp; UPPER(LEFT(stand_md!AC2,3)) &amp; IF(ISBLANK(stand_md!AC4),"","_") &amp; UPPER(LEFT(stand_md!AC4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AC$3,1) &amp; RIGHT(plant_md!AC$3,LEN(plant_md!AC$3)-FIND(" ",plant_md!AC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AC$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AC$3,1) &amp; RIGHT(plant_md!AC$3,LEN(plant_md!AC$3)-FIND(" ",plant_md!AC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AC$1,"")</f>
         <v/>
       </c>
       <c r="AD25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AD2),"","_") &amp; UPPER(LEFT(stand_md!AD2,3)) &amp; IF(ISBLANK(stand_md!AD4),"","_") &amp; UPPER(LEFT(stand_md!AD4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AD$3,1) &amp; RIGHT(plant_md!AD$3,LEN(plant_md!AD$3)-FIND(" ",plant_md!AD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AD$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AD$3,1) &amp; RIGHT(plant_md!AD$3,LEN(plant_md!AD$3)-FIND(" ",plant_md!AD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AD$1,"")</f>
         <v/>
       </c>
       <c r="AE25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AE2),"","_") &amp; UPPER(LEFT(stand_md!AE2,3)) &amp; IF(ISBLANK(stand_md!AE4),"","_") &amp; UPPER(LEFT(stand_md!AE4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AE$3,1) &amp; RIGHT(plant_md!AE$3,LEN(plant_md!AE$3)-FIND(" ",plant_md!AE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AE$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AE$3,1) &amp; RIGHT(plant_md!AE$3,LEN(plant_md!AE$3)-FIND(" ",plant_md!AE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AE$1,"")</f>
         <v/>
       </c>
       <c r="AF25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AF2),"","_") &amp; UPPER(LEFT(stand_md!AF2,3)) &amp; IF(ISBLANK(stand_md!AF4),"","_") &amp; UPPER(LEFT(stand_md!AF4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AF$3,1) &amp; RIGHT(plant_md!AF$3,LEN(plant_md!AF$3)-FIND(" ",plant_md!AF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AF$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AF$3,1) &amp; RIGHT(plant_md!AF$3,LEN(plant_md!AF$3)-FIND(" ",plant_md!AF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AF$1,"")</f>
         <v/>
       </c>
       <c r="AG25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AG2),"","_") &amp; UPPER(LEFT(stand_md!AG2,3)) &amp; IF(ISBLANK(stand_md!AG4),"","_") &amp; UPPER(LEFT(stand_md!AG4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AG$3,1) &amp; RIGHT(plant_md!AG$3,LEN(plant_md!AG$3)-FIND(" ",plant_md!AG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AG$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AG$3,1) &amp; RIGHT(plant_md!AG$3,LEN(plant_md!AG$3)-FIND(" ",plant_md!AG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AG$1,"")</f>
         <v/>
       </c>
       <c r="AH25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AH2),"","_") &amp; UPPER(LEFT(stand_md!AH2,3)) &amp; IF(ISBLANK(stand_md!AH4),"","_") &amp; UPPER(LEFT(stand_md!AH4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AH$3,1) &amp; RIGHT(plant_md!AH$3,LEN(plant_md!AH$3)-FIND(" ",plant_md!AH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AH$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AH$3,1) &amp; RIGHT(plant_md!AH$3,LEN(plant_md!AH$3)-FIND(" ",plant_md!AH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AH$1,"")</f>
         <v/>
       </c>
       <c r="AI25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AI2),"","_") &amp; UPPER(LEFT(stand_md!AI2,3)) &amp; IF(ISBLANK(stand_md!AI4),"","_") &amp; UPPER(LEFT(stand_md!AI4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AI$3,1) &amp; RIGHT(plant_md!AI$3,LEN(plant_md!AI$3)-FIND(" ",plant_md!AI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AI$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AI$3,1) &amp; RIGHT(plant_md!AI$3,LEN(plant_md!AI$3)-FIND(" ",plant_md!AI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AI$1,"")</f>
         <v/>
       </c>
       <c r="AJ25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AJ2),"","_") &amp; UPPER(LEFT(stand_md!AJ2,3)) &amp; IF(ISBLANK(stand_md!AJ4),"","_") &amp; UPPER(LEFT(stand_md!AJ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AJ$3,1) &amp; RIGHT(plant_md!AJ$3,LEN(plant_md!AJ$3)-FIND(" ",plant_md!AJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AJ$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AJ$3,1) &amp; RIGHT(plant_md!AJ$3,LEN(plant_md!AJ$3)-FIND(" ",plant_md!AJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AJ$1,"")</f>
         <v/>
       </c>
       <c r="AK25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AK2),"","_") &amp; UPPER(LEFT(stand_md!AK2,3)) &amp; IF(ISBLANK(stand_md!AK4),"","_") &amp; UPPER(LEFT(stand_md!AK4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AK$3,1) &amp; RIGHT(plant_md!AK$3,LEN(plant_md!AK$3)-FIND(" ",plant_md!AK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AK$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AK$3,1) &amp; RIGHT(plant_md!AK$3,LEN(plant_md!AK$3)-FIND(" ",plant_md!AK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AK$1,"")</f>
         <v/>
       </c>
       <c r="AL25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AL2),"","_") &amp; UPPER(LEFT(stand_md!AL2,3)) &amp; IF(ISBLANK(stand_md!AL4),"","_") &amp; UPPER(LEFT(stand_md!AL4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AL$3,1) &amp; RIGHT(plant_md!AL$3,LEN(plant_md!AL$3)-FIND(" ",plant_md!AL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AL$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AL$3,1) &amp; RIGHT(plant_md!AL$3,LEN(plant_md!AL$3)-FIND(" ",plant_md!AL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AL$1,"")</f>
         <v/>
       </c>
       <c r="AM25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AM2),"","_") &amp; UPPER(LEFT(stand_md!AM2,3)) &amp; IF(ISBLANK(stand_md!AM4),"","_") &amp; UPPER(LEFT(stand_md!AM4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AM$3,1) &amp; RIGHT(plant_md!AM$3,LEN(plant_md!AM$3)-FIND(" ",plant_md!AM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AM$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AM$3,1) &amp; RIGHT(plant_md!AM$3,LEN(plant_md!AM$3)-FIND(" ",plant_md!AM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AM$1,"")</f>
         <v/>
       </c>
       <c r="AN25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AN2),"","_") &amp; UPPER(LEFT(stand_md!AN2,3)) &amp; IF(ISBLANK(stand_md!AN4),"","_") &amp; UPPER(LEFT(stand_md!AN4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AN$3,1) &amp; RIGHT(plant_md!AN$3,LEN(plant_md!AN$3)-FIND(" ",plant_md!AN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AN$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AN$3,1) &amp; RIGHT(plant_md!AN$3,LEN(plant_md!AN$3)-FIND(" ",plant_md!AN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AN$1,"")</f>
         <v/>
       </c>
       <c r="AO25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AO2),"","_") &amp; UPPER(LEFT(stand_md!AO2,3)) &amp; IF(ISBLANK(stand_md!AO4),"","_") &amp; UPPER(LEFT(stand_md!AO4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AO$3,1) &amp; RIGHT(plant_md!AO$3,LEN(plant_md!AO$3)-FIND(" ",plant_md!AO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AO$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AO$3,1) &amp; RIGHT(plant_md!AO$3,LEN(plant_md!AO$3)-FIND(" ",plant_md!AO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AO$1,"")</f>
         <v/>
       </c>
       <c r="AP25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AP2),"","_") &amp; UPPER(LEFT(stand_md!AP2,3)) &amp; IF(ISBLANK(stand_md!AP4),"","_") &amp; UPPER(LEFT(stand_md!AP4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AP$3,1) &amp; RIGHT(plant_md!AP$3,LEN(plant_md!AP$3)-FIND(" ",plant_md!AP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AP$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AP$3,1) &amp; RIGHT(plant_md!AP$3,LEN(plant_md!AP$3)-FIND(" ",plant_md!AP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AP$1,"")</f>
         <v/>
       </c>
       <c r="AQ25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AQ2),"","_") &amp; UPPER(LEFT(stand_md!AQ2,3)) &amp; IF(ISBLANK(stand_md!AQ4),"","_") &amp; UPPER(LEFT(stand_md!AQ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AQ$3,1) &amp; RIGHT(plant_md!AQ$3,LEN(plant_md!AQ$3)-FIND(" ",plant_md!AQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AQ$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AQ$3,1) &amp; RIGHT(plant_md!AQ$3,LEN(plant_md!AQ$3)-FIND(" ",plant_md!AQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AQ$1,"")</f>
         <v/>
       </c>
       <c r="AR25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AR2),"","_") &amp; UPPER(LEFT(stand_md!AR2,3)) &amp; IF(ISBLANK(stand_md!AR4),"","_") &amp; UPPER(LEFT(stand_md!AR4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AR$3,1) &amp; RIGHT(plant_md!AR$3,LEN(plant_md!AR$3)-FIND(" ",plant_md!AR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AR$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AR$3,1) &amp; RIGHT(plant_md!AR$3,LEN(plant_md!AR$3)-FIND(" ",plant_md!AR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AR$1,"")</f>
         <v/>
       </c>
       <c r="AS25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AS2),"","_") &amp; UPPER(LEFT(stand_md!AS2,3)) &amp; IF(ISBLANK(stand_md!AS4),"","_") &amp; UPPER(LEFT(stand_md!AS4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AS$3,1) &amp; RIGHT(plant_md!AS$3,LEN(plant_md!AS$3)-FIND(" ",plant_md!AS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AS$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AS$3,1) &amp; RIGHT(plant_md!AS$3,LEN(plant_md!AS$3)-FIND(" ",plant_md!AS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AS$1,"")</f>
         <v/>
       </c>
       <c r="AT25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AT2),"","_") &amp; UPPER(LEFT(stand_md!AT2,3)) &amp; IF(ISBLANK(stand_md!AT4),"","_") &amp; UPPER(LEFT(stand_md!AT4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AT$3,1) &amp; RIGHT(plant_md!AT$3,LEN(plant_md!AT$3)-FIND(" ",plant_md!AT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AT$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AT$3,1) &amp; RIGHT(plant_md!AT$3,LEN(plant_md!AT$3)-FIND(" ",plant_md!AT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AT$1,"")</f>
         <v/>
       </c>
       <c r="AU25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AU2),"","_") &amp; UPPER(LEFT(stand_md!AU2,3)) &amp; IF(ISBLANK(stand_md!AU4),"","_") &amp; UPPER(LEFT(stand_md!AU4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AU$3,1) &amp; RIGHT(plant_md!AU$3,LEN(plant_md!AU$3)-FIND(" ",plant_md!AU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AU$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AU$3,1) &amp; RIGHT(plant_md!AU$3,LEN(plant_md!AU$3)-FIND(" ",plant_md!AU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AU$1,"")</f>
         <v/>
       </c>
       <c r="AV25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AV2),"","_") &amp; UPPER(LEFT(stand_md!AV2,3)) &amp; IF(ISBLANK(stand_md!AV4),"","_") &amp; UPPER(LEFT(stand_md!AV4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AV$3,1) &amp; RIGHT(plant_md!AV$3,LEN(plant_md!AV$3)-FIND(" ",plant_md!AV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AV$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AV$3,1) &amp; RIGHT(plant_md!AV$3,LEN(plant_md!AV$3)-FIND(" ",plant_md!AV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AV$1,"")</f>
         <v/>
       </c>
       <c r="AW25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AW2),"","_") &amp; UPPER(LEFT(stand_md!AW2,3)) &amp; IF(ISBLANK(stand_md!AW4),"","_") &amp; UPPER(LEFT(stand_md!AW4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AW$3,1) &amp; RIGHT(plant_md!AW$3,LEN(plant_md!AW$3)-FIND(" ",plant_md!AW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AW$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AW$3,1) &amp; RIGHT(plant_md!AW$3,LEN(plant_md!AW$3)-FIND(" ",plant_md!AW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AW$1,"")</f>
         <v/>
       </c>
       <c r="AX25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AX2),"","_") &amp; UPPER(LEFT(stand_md!AX2,3)) &amp; IF(ISBLANK(stand_md!AX4),"","_") &amp; UPPER(LEFT(stand_md!AX4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AX$3,1) &amp; RIGHT(plant_md!AX$3,LEN(plant_md!AX$3)-FIND(" ",plant_md!AX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AX$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AX$3,1) &amp; RIGHT(plant_md!AX$3,LEN(plant_md!AX$3)-FIND(" ",plant_md!AX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AX$1,"")</f>
         <v/>
       </c>
       <c r="AY25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AY2),"","_") &amp; UPPER(LEFT(stand_md!AY2,3)) &amp; IF(ISBLANK(stand_md!AY4),"","_") &amp; UPPER(LEFT(stand_md!AY4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AY$3,1) &amp; RIGHT(plant_md!AY$3,LEN(plant_md!AY$3)-FIND(" ",plant_md!AY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AY$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AY$3,1) &amp; RIGHT(plant_md!AY$3,LEN(plant_md!AY$3)-FIND(" ",plant_md!AY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AY$1,"")</f>
         <v/>
       </c>
       <c r="AZ25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AZ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AZ2),"","_") &amp; UPPER(LEFT(stand_md!AZ2,3)) &amp; IF(ISBLANK(stand_md!AZ4),"","_") &amp; UPPER(LEFT(stand_md!AZ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AZ$3,1) &amp; RIGHT(plant_md!AZ$3,LEN(plant_md!AZ$3)-FIND(" ",plant_md!AZ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AZ$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AZ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AZ$3,1) &amp; RIGHT(plant_md!AZ$3,LEN(plant_md!AZ$3)-FIND(" ",plant_md!AZ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AZ$1,"")</f>
         <v/>
       </c>
       <c r="BA25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BA2),"","_") &amp; UPPER(LEFT(stand_md!BA2,3)) &amp; IF(ISBLANK(stand_md!BA4),"","_") &amp; UPPER(LEFT(stand_md!BA4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BA$3,1) &amp; RIGHT(plant_md!BA$3,LEN(plant_md!BA$3)-FIND(" ",plant_md!BA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BA$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BA$3,1) &amp; RIGHT(plant_md!BA$3,LEN(plant_md!BA$3)-FIND(" ",plant_md!BA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BA$1,"")</f>
         <v/>
       </c>
       <c r="BB25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BB2),"","_") &amp; UPPER(LEFT(stand_md!BB2,3)) &amp; IF(ISBLANK(stand_md!BB4),"","_") &amp; UPPER(LEFT(stand_md!BB4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BB$3,1) &amp; RIGHT(plant_md!BB$3,LEN(plant_md!BB$3)-FIND(" ",plant_md!BB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BB$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BB$3,1) &amp; RIGHT(plant_md!BB$3,LEN(plant_md!BB$3)-FIND(" ",plant_md!BB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BB$1,"")</f>
         <v/>
       </c>
       <c r="BC25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BC2),"","_") &amp; UPPER(LEFT(stand_md!BC2,3)) &amp; IF(ISBLANK(stand_md!BC4),"","_") &amp; UPPER(LEFT(stand_md!BC4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BC$3,1) &amp; RIGHT(plant_md!BC$3,LEN(plant_md!BC$3)-FIND(" ",plant_md!BC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BC$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BC$3,1) &amp; RIGHT(plant_md!BC$3,LEN(plant_md!BC$3)-FIND(" ",plant_md!BC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BC$1,"")</f>
         <v/>
       </c>
       <c r="BD25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BD2),"","_") &amp; UPPER(LEFT(stand_md!BD2,3)) &amp; IF(ISBLANK(stand_md!BD4),"","_") &amp; UPPER(LEFT(stand_md!BD4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BD$3,1) &amp; RIGHT(plant_md!BD$3,LEN(plant_md!BD$3)-FIND(" ",plant_md!BD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BD$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BD$3,1) &amp; RIGHT(plant_md!BD$3,LEN(plant_md!BD$3)-FIND(" ",plant_md!BD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BD$1,"")</f>
         <v/>
       </c>
       <c r="BE25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BE2),"","_") &amp; UPPER(LEFT(stand_md!BE2,3)) &amp; IF(ISBLANK(stand_md!BE4),"","_") &amp; UPPER(LEFT(stand_md!BE4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BE$3,1) &amp; RIGHT(plant_md!BE$3,LEN(plant_md!BE$3)-FIND(" ",plant_md!BE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BE$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BE$3,1) &amp; RIGHT(plant_md!BE$3,LEN(plant_md!BE$3)-FIND(" ",plant_md!BE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BE$1,"")</f>
         <v/>
       </c>
       <c r="BF25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BF2),"","_") &amp; UPPER(LEFT(stand_md!BF2,3)) &amp; IF(ISBLANK(stand_md!BF4),"","_") &amp; UPPER(LEFT(stand_md!BF4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BF$3,1) &amp; RIGHT(plant_md!BF$3,LEN(plant_md!BF$3)-FIND(" ",plant_md!BF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BF$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BF$3,1) &amp; RIGHT(plant_md!BF$3,LEN(plant_md!BF$3)-FIND(" ",plant_md!BF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BF$1,"")</f>
         <v/>
       </c>
       <c r="BG25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BG2),"","_") &amp; UPPER(LEFT(stand_md!BG2,3)) &amp; IF(ISBLANK(stand_md!BG4),"","_") &amp; UPPER(LEFT(stand_md!BG4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BG$3,1) &amp; RIGHT(plant_md!BG$3,LEN(plant_md!BG$3)-FIND(" ",plant_md!BG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BG$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BG$3,1) &amp; RIGHT(plant_md!BG$3,LEN(plant_md!BG$3)-FIND(" ",plant_md!BG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BG$1,"")</f>
         <v/>
       </c>
       <c r="BH25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BH2),"","_") &amp; UPPER(LEFT(stand_md!BH2,3)) &amp; IF(ISBLANK(stand_md!BH4),"","_") &amp; UPPER(LEFT(stand_md!BH4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BH$3,1) &amp; RIGHT(plant_md!BH$3,LEN(plant_md!BH$3)-FIND(" ",plant_md!BH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BH$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BH$3,1) &amp; RIGHT(plant_md!BH$3,LEN(plant_md!BH$3)-FIND(" ",plant_md!BH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BH$1,"")</f>
         <v/>
       </c>
       <c r="BI25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BI2),"","_") &amp; UPPER(LEFT(stand_md!BI2,3)) &amp; IF(ISBLANK(stand_md!BI4),"","_") &amp; UPPER(LEFT(stand_md!BI4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BI$3,1) &amp; RIGHT(plant_md!BI$3,LEN(plant_md!BI$3)-FIND(" ",plant_md!BI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BI$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BI$3,1) &amp; RIGHT(plant_md!BI$3,LEN(plant_md!BI$3)-FIND(" ",plant_md!BI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BI$1,"")</f>
         <v/>
       </c>
       <c r="BJ25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BJ2),"","_") &amp; UPPER(LEFT(stand_md!BJ2,3)) &amp; IF(ISBLANK(stand_md!BJ4),"","_") &amp; UPPER(LEFT(stand_md!BJ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BJ$3,1) &amp; RIGHT(plant_md!BJ$3,LEN(plant_md!BJ$3)-FIND(" ",plant_md!BJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BJ$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BJ$3,1) &amp; RIGHT(plant_md!BJ$3,LEN(plant_md!BJ$3)-FIND(" ",plant_md!BJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BJ$1,"")</f>
         <v/>
       </c>
       <c r="BK25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BK2),"","_") &amp; UPPER(LEFT(stand_md!BK2,3)) &amp; IF(ISBLANK(stand_md!BK4),"","_") &amp; UPPER(LEFT(stand_md!BK4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BK$3,1) &amp; RIGHT(plant_md!BK$3,LEN(plant_md!BK$3)-FIND(" ",plant_md!BK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BK$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BK$3,1) &amp; RIGHT(plant_md!BK$3,LEN(plant_md!BK$3)-FIND(" ",plant_md!BK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BK$1,"")</f>
         <v/>
       </c>
       <c r="BL25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BL2),"","_") &amp; UPPER(LEFT(stand_md!BL2,3)) &amp; IF(ISBLANK(stand_md!BL4),"","_") &amp; UPPER(LEFT(stand_md!BL4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BL$3,1) &amp; RIGHT(plant_md!BL$3,LEN(plant_md!BL$3)-FIND(" ",plant_md!BL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BL$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BL$3,1) &amp; RIGHT(plant_md!BL$3,LEN(plant_md!BL$3)-FIND(" ",plant_md!BL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BL$1,"")</f>
         <v/>
       </c>
       <c r="BM25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BM2),"","_") &amp; UPPER(LEFT(stand_md!BM2,3)) &amp; IF(ISBLANK(stand_md!BM4),"","_") &amp; UPPER(LEFT(stand_md!BM4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BM$3,1) &amp; RIGHT(plant_md!BM$3,LEN(plant_md!BM$3)-FIND(" ",plant_md!BM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BM$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BM$3,1) &amp; RIGHT(plant_md!BM$3,LEN(plant_md!BM$3)-FIND(" ",plant_md!BM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BM$1,"")</f>
         <v/>
       </c>
       <c r="BN25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BN2),"","_") &amp; UPPER(LEFT(stand_md!BN2,3)) &amp; IF(ISBLANK(stand_md!BN4),"","_") &amp; UPPER(LEFT(stand_md!BN4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BN$3,1) &amp; RIGHT(plant_md!BN$3,LEN(plant_md!BN$3)-FIND(" ",plant_md!BN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BN$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BN$3,1) &amp; RIGHT(plant_md!BN$3,LEN(plant_md!BN$3)-FIND(" ",plant_md!BN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BN$1,"")</f>
         <v/>
       </c>
       <c r="BO25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BO2),"","_") &amp; UPPER(LEFT(stand_md!BO2,3)) &amp; IF(ISBLANK(stand_md!BO4),"","_") &amp; UPPER(LEFT(stand_md!BO4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BO$3,1) &amp; RIGHT(plant_md!BO$3,LEN(plant_md!BO$3)-FIND(" ",plant_md!BO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BO$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BO$3,1) &amp; RIGHT(plant_md!BO$3,LEN(plant_md!BO$3)-FIND(" ",plant_md!BO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BO$1,"")</f>
         <v/>
       </c>
       <c r="BP25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BP2),"","_") &amp; UPPER(LEFT(stand_md!BP2,3)) &amp; IF(ISBLANK(stand_md!BP4),"","_") &amp; UPPER(LEFT(stand_md!BP4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BP$3,1) &amp; RIGHT(plant_md!BP$3,LEN(plant_md!BP$3)-FIND(" ",plant_md!BP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BP$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BP$3,1) &amp; RIGHT(plant_md!BP$3,LEN(plant_md!BP$3)-FIND(" ",plant_md!BP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BP$1,"")</f>
         <v/>
       </c>
       <c r="BQ25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BQ2),"","_") &amp; UPPER(LEFT(stand_md!BQ2,3)) &amp; IF(ISBLANK(stand_md!BQ4),"","_") &amp; UPPER(LEFT(stand_md!BQ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BQ$3,1) &amp; RIGHT(plant_md!BQ$3,LEN(plant_md!BQ$3)-FIND(" ",plant_md!BQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BQ$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BQ$3,1) &amp; RIGHT(plant_md!BQ$3,LEN(plant_md!BQ$3)-FIND(" ",plant_md!BQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BQ$1,"")</f>
         <v/>
       </c>
       <c r="BR25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BR2),"","_") &amp; UPPER(LEFT(stand_md!BR2,3)) &amp; IF(ISBLANK(stand_md!BR4),"","_") &amp; UPPER(LEFT(stand_md!BR4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BR$3,1) &amp; RIGHT(plant_md!BR$3,LEN(plant_md!BR$3)-FIND(" ",plant_md!BR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BR$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BR$3,1) &amp; RIGHT(plant_md!BR$3,LEN(plant_md!BR$3)-FIND(" ",plant_md!BR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BR$1,"")</f>
         <v/>
       </c>
       <c r="BS25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BS2),"","_") &amp; UPPER(LEFT(stand_md!BS2,3)) &amp; IF(ISBLANK(stand_md!BS4),"","_") &amp; UPPER(LEFT(stand_md!BS4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BS$3,1) &amp; RIGHT(plant_md!BS$3,LEN(plant_md!BS$3)-FIND(" ",plant_md!BS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BS$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BS$3,1) &amp; RIGHT(plant_md!BS$3,LEN(plant_md!BS$3)-FIND(" ",plant_md!BS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BS$1,"")</f>
         <v/>
       </c>
       <c r="BT25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BT2),"","_") &amp; UPPER(LEFT(stand_md!BT2,3)) &amp; IF(ISBLANK(stand_md!BT4),"","_") &amp; UPPER(LEFT(stand_md!BT4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BT$3,1) &amp; RIGHT(plant_md!BT$3,LEN(plant_md!BT$3)-FIND(" ",plant_md!BT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BT$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BT$3,1) &amp; RIGHT(plant_md!BT$3,LEN(plant_md!BT$3)-FIND(" ",plant_md!BT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BT$1,"")</f>
         <v/>
       </c>
       <c r="BU25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BU2),"","_") &amp; UPPER(LEFT(stand_md!BU2,3)) &amp; IF(ISBLANK(stand_md!BU4),"","_") &amp; UPPER(LEFT(stand_md!BU4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BU$3,1) &amp; RIGHT(plant_md!BU$3,LEN(plant_md!BU$3)-FIND(" ",plant_md!BU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BU$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BU$3,1) &amp; RIGHT(plant_md!BU$3,LEN(plant_md!BU$3)-FIND(" ",plant_md!BU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BU$1,"")</f>
         <v/>
       </c>
       <c r="BV25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BV2),"","_") &amp; UPPER(LEFT(stand_md!BV2,3)) &amp; IF(ISBLANK(stand_md!BV4),"","_") &amp; UPPER(LEFT(stand_md!BV4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BV$3,1) &amp; RIGHT(plant_md!BV$3,LEN(plant_md!BV$3)-FIND(" ",plant_md!BV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BV$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BV$3,1) &amp; RIGHT(plant_md!BV$3,LEN(plant_md!BV$3)-FIND(" ",plant_md!BV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BV$1,"")</f>
         <v/>
       </c>
       <c r="BW25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BW2),"","_") &amp; UPPER(LEFT(stand_md!BW2,3)) &amp; IF(ISBLANK(stand_md!BW4),"","_") &amp; UPPER(LEFT(stand_md!BW4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BW$3,1) &amp; RIGHT(plant_md!BW$3,LEN(plant_md!BW$3)-FIND(" ",plant_md!BW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BW$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BW$3,1) &amp; RIGHT(plant_md!BW$3,LEN(plant_md!BW$3)-FIND(" ",plant_md!BW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BW$1,"")</f>
         <v/>
       </c>
       <c r="BX25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BX2),"","_") &amp; UPPER(LEFT(stand_md!BX2,3)) &amp; IF(ISBLANK(stand_md!BX4),"","_") &amp; UPPER(LEFT(stand_md!BX4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BX$3,1) &amp; RIGHT(plant_md!BX$3,LEN(plant_md!BX$3)-FIND(" ",plant_md!BX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BX$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BX$3,1) &amp; RIGHT(plant_md!BX$3,LEN(plant_md!BX$3)-FIND(" ",plant_md!BX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BX$1,"")</f>
         <v/>
       </c>
       <c r="BY25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BY2),"","_") &amp; UPPER(LEFT(stand_md!BY2,3)) &amp; IF(ISBLANK(stand_md!BY4),"","_") &amp; UPPER(LEFT(stand_md!BY4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BY$3,1) &amp; RIGHT(plant_md!BY$3,LEN(plant_md!BY$3)-FIND(" ",plant_md!BY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BY$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BY$3,1) &amp; RIGHT(plant_md!BY$3,LEN(plant_md!BY$3)-FIND(" ",plant_md!BY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BY$1,"")</f>
         <v/>
       </c>
       <c r="BZ25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BZ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BZ2),"","_") &amp; UPPER(LEFT(stand_md!BZ2,3)) &amp; IF(ISBLANK(stand_md!BZ4),"","_") &amp; UPPER(LEFT(stand_md!BZ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BZ$3,1) &amp; RIGHT(plant_md!BZ$3,LEN(plant_md!BZ$3)-FIND(" ",plant_md!BZ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BZ$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BZ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BZ$3,1) &amp; RIGHT(plant_md!BZ$3,LEN(plant_md!BZ$3)-FIND(" ",plant_md!BZ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BZ$1,"")</f>
         <v/>
       </c>
       <c r="CA25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CA2),"","_") &amp; UPPER(LEFT(stand_md!CA2,3)) &amp; IF(ISBLANK(stand_md!CA4),"","_") &amp; UPPER(LEFT(stand_md!CA4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CA$3,1) &amp; RIGHT(plant_md!CA$3,LEN(plant_md!CA$3)-FIND(" ",plant_md!CA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CA$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CA$3,1) &amp; RIGHT(plant_md!CA$3,LEN(plant_md!CA$3)-FIND(" ",plant_md!CA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CA$1,"")</f>
         <v/>
       </c>
       <c r="CB25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CB2),"","_") &amp; UPPER(LEFT(stand_md!CB2,3)) &amp; IF(ISBLANK(stand_md!CB4),"","_") &amp; UPPER(LEFT(stand_md!CB4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CB$3,1) &amp; RIGHT(plant_md!CB$3,LEN(plant_md!CB$3)-FIND(" ",plant_md!CB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CB$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CB$3,1) &amp; RIGHT(plant_md!CB$3,LEN(plant_md!CB$3)-FIND(" ",plant_md!CB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CB$1,"")</f>
         <v/>
       </c>
       <c r="CC25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CC2),"","_") &amp; UPPER(LEFT(stand_md!CC2,3)) &amp; IF(ISBLANK(stand_md!CC4),"","_") &amp; UPPER(LEFT(stand_md!CC4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CC$3,1) &amp; RIGHT(plant_md!CC$3,LEN(plant_md!CC$3)-FIND(" ",plant_md!CC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CC$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CC$3,1) &amp; RIGHT(plant_md!CC$3,LEN(plant_md!CC$3)-FIND(" ",plant_md!CC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CC$1,"")</f>
         <v/>
       </c>
       <c r="CD25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CD2),"","_") &amp; UPPER(LEFT(stand_md!CD2,3)) &amp; IF(ISBLANK(stand_md!CD4),"","_") &amp; UPPER(LEFT(stand_md!CD4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CD$3,1) &amp; RIGHT(plant_md!CD$3,LEN(plant_md!CD$3)-FIND(" ",plant_md!CD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CD$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CD$3,1) &amp; RIGHT(plant_md!CD$3,LEN(plant_md!CD$3)-FIND(" ",plant_md!CD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CD$1,"")</f>
         <v/>
       </c>
       <c r="CE25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CE2),"","_") &amp; UPPER(LEFT(stand_md!CE2,3)) &amp; IF(ISBLANK(stand_md!CE4),"","_") &amp; UPPER(LEFT(stand_md!CE4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CE$3,1) &amp; RIGHT(plant_md!CE$3,LEN(plant_md!CE$3)-FIND(" ",plant_md!CE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CE$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CE$3,1) &amp; RIGHT(plant_md!CE$3,LEN(plant_md!CE$3)-FIND(" ",plant_md!CE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CE$1,"")</f>
         <v/>
       </c>
       <c r="CF25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CF2),"","_") &amp; UPPER(LEFT(stand_md!CF2,3)) &amp; IF(ISBLANK(stand_md!CF4),"","_") &amp; UPPER(LEFT(stand_md!CF4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CF$3,1) &amp; RIGHT(plant_md!CF$3,LEN(plant_md!CF$3)-FIND(" ",plant_md!CF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CF$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CF$3,1) &amp; RIGHT(plant_md!CF$3,LEN(plant_md!CF$3)-FIND(" ",plant_md!CF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CF$1,"")</f>
         <v/>
       </c>
       <c r="CG25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CG2),"","_") &amp; UPPER(LEFT(stand_md!CG2,3)) &amp; IF(ISBLANK(stand_md!CG4),"","_") &amp; UPPER(LEFT(stand_md!CG4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CG$3,1) &amp; RIGHT(plant_md!CG$3,LEN(plant_md!CG$3)-FIND(" ",plant_md!CG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CG$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CG$3,1) &amp; RIGHT(plant_md!CG$3,LEN(plant_md!CG$3)-FIND(" ",plant_md!CG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CG$1,"")</f>
         <v/>
       </c>
       <c r="CH25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CH2),"","_") &amp; UPPER(LEFT(stand_md!CH2,3)) &amp; IF(ISBLANK(stand_md!CH4),"","_") &amp; UPPER(LEFT(stand_md!CH4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CH$3,1) &amp; RIGHT(plant_md!CH$3,LEN(plant_md!CH$3)-FIND(" ",plant_md!CH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CH$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CH$3,1) &amp; RIGHT(plant_md!CH$3,LEN(plant_md!CH$3)-FIND(" ",plant_md!CH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CH$1,"")</f>
         <v/>
       </c>
       <c r="CI25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CI2),"","_") &amp; UPPER(LEFT(stand_md!CI2,3)) &amp; IF(ISBLANK(stand_md!CI4),"","_") &amp; UPPER(LEFT(stand_md!CI4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CI$3,1) &amp; RIGHT(plant_md!CI$3,LEN(plant_md!CI$3)-FIND(" ",plant_md!CI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CI$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CI$3,1) &amp; RIGHT(plant_md!CI$3,LEN(plant_md!CI$3)-FIND(" ",plant_md!CI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CI$1,"")</f>
         <v/>
       </c>
       <c r="CJ25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CJ2),"","_") &amp; UPPER(LEFT(stand_md!CJ2,3)) &amp; IF(ISBLANK(stand_md!CJ4),"","_") &amp; UPPER(LEFT(stand_md!CJ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CJ$3,1) &amp; RIGHT(plant_md!CJ$3,LEN(plant_md!CJ$3)-FIND(" ",plant_md!CJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CJ$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CJ$3,1) &amp; RIGHT(plant_md!CJ$3,LEN(plant_md!CJ$3)-FIND(" ",plant_md!CJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CJ$1,"")</f>
         <v/>
       </c>
       <c r="CK25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CK2),"","_") &amp; UPPER(LEFT(stand_md!CK2,3)) &amp; IF(ISBLANK(stand_md!CK4),"","_") &amp; UPPER(LEFT(stand_md!CK4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CK$3,1) &amp; RIGHT(plant_md!CK$3,LEN(plant_md!CK$3)-FIND(" ",plant_md!CK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CK$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CK$3,1) &amp; RIGHT(plant_md!CK$3,LEN(plant_md!CK$3)-FIND(" ",plant_md!CK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CK$1,"")</f>
         <v/>
       </c>
       <c r="CL25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CL2),"","_") &amp; UPPER(LEFT(stand_md!CL2,3)) &amp; IF(ISBLANK(stand_md!CL4),"","_") &amp; UPPER(LEFT(stand_md!CL4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CL$3,1) &amp; RIGHT(plant_md!CL$3,LEN(plant_md!CL$3)-FIND(" ",plant_md!CL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CL$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CL$3,1) &amp; RIGHT(plant_md!CL$3,LEN(plant_md!CL$3)-FIND(" ",plant_md!CL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CL$1,"")</f>
         <v/>
       </c>
       <c r="CM25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CM2),"","_") &amp; UPPER(LEFT(stand_md!CM2,3)) &amp; IF(ISBLANK(stand_md!CM4),"","_") &amp; UPPER(LEFT(stand_md!CM4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CM$3,1) &amp; RIGHT(plant_md!CM$3,LEN(plant_md!CM$3)-FIND(" ",plant_md!CM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CM$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CM$3,1) &amp; RIGHT(plant_md!CM$3,LEN(plant_md!CM$3)-FIND(" ",plant_md!CM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CM$1,"")</f>
         <v/>
       </c>
       <c r="CN25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CN2),"","_") &amp; UPPER(LEFT(stand_md!CN2,3)) &amp; IF(ISBLANK(stand_md!CN4),"","_") &amp; UPPER(LEFT(stand_md!CN4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CN$3,1) &amp; RIGHT(plant_md!CN$3,LEN(plant_md!CN$3)-FIND(" ",plant_md!CN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CN$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CN$3,1) &amp; RIGHT(plant_md!CN$3,LEN(plant_md!CN$3)-FIND(" ",plant_md!CN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CN$1,"")</f>
         <v/>
       </c>
       <c r="CO25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CO2),"","_") &amp; UPPER(LEFT(stand_md!CO2,3)) &amp; IF(ISBLANK(stand_md!CO4),"","_") &amp; UPPER(LEFT(stand_md!CO4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CO$3,1) &amp; RIGHT(plant_md!CO$3,LEN(plant_md!CO$3)-FIND(" ",plant_md!CO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CO$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CO$3,1) &amp; RIGHT(plant_md!CO$3,LEN(plant_md!CO$3)-FIND(" ",plant_md!CO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CO$1,"")</f>
         <v/>
       </c>
       <c r="CP25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CP2),"","_") &amp; UPPER(LEFT(stand_md!CP2,3)) &amp; IF(ISBLANK(stand_md!CP4),"","_") &amp; UPPER(LEFT(stand_md!CP4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CP$3,1) &amp; RIGHT(plant_md!CP$3,LEN(plant_md!CP$3)-FIND(" ",plant_md!CP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CP$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CP$3,1) &amp; RIGHT(plant_md!CP$3,LEN(plant_md!CP$3)-FIND(" ",plant_md!CP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CP$1,"")</f>
         <v/>
       </c>
       <c r="CQ25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CQ2),"","_") &amp; UPPER(LEFT(stand_md!CQ2,3)) &amp; IF(ISBLANK(stand_md!CQ4),"","_") &amp; UPPER(LEFT(stand_md!CQ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CQ$3,1) &amp; RIGHT(plant_md!CQ$3,LEN(plant_md!CQ$3)-FIND(" ",plant_md!CQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CQ$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CQ$3,1) &amp; RIGHT(plant_md!CQ$3,LEN(plant_md!CQ$3)-FIND(" ",plant_md!CQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CQ$1,"")</f>
         <v/>
       </c>
       <c r="CR25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CR2),"","_") &amp; UPPER(LEFT(stand_md!CR2,3)) &amp; IF(ISBLANK(stand_md!CR4),"","_") &amp; UPPER(LEFT(stand_md!CR4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CR$3,1) &amp; RIGHT(plant_md!CR$3,LEN(plant_md!CR$3)-FIND(" ",plant_md!CR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CR$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CR$3,1) &amp; RIGHT(plant_md!CR$3,LEN(plant_md!CR$3)-FIND(" ",plant_md!CR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CR$1,"")</f>
         <v/>
       </c>
       <c r="CS25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CS2),"","_") &amp; UPPER(LEFT(stand_md!CS2,3)) &amp; IF(ISBLANK(stand_md!CS4),"","_") &amp; UPPER(LEFT(stand_md!CS4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CS$3,1) &amp; RIGHT(plant_md!CS$3,LEN(plant_md!CS$3)-FIND(" ",plant_md!CS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CS$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CS$3,1) &amp; RIGHT(plant_md!CS$3,LEN(plant_md!CS$3)-FIND(" ",plant_md!CS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CS$1,"")</f>
         <v/>
       </c>
       <c r="CT25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CT2),"","_") &amp; UPPER(LEFT(stand_md!CT2,3)) &amp; IF(ISBLANK(stand_md!CT4),"","_") &amp; UPPER(LEFT(stand_md!CT4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CT$3,1) &amp; RIGHT(plant_md!CT$3,LEN(plant_md!CT$3)-FIND(" ",plant_md!CT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CT$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CT$3,1) &amp; RIGHT(plant_md!CT$3,LEN(plant_md!CT$3)-FIND(" ",plant_md!CT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CT$1,"")</f>
         <v/>
       </c>
       <c r="CU25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CU2),"","_") &amp; UPPER(LEFT(stand_md!CU2,3)) &amp; IF(ISBLANK(stand_md!CU4),"","_") &amp; UPPER(LEFT(stand_md!CU4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CU$3,1) &amp; RIGHT(plant_md!CU$3,LEN(plant_md!CU$3)-FIND(" ",plant_md!CU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CU$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CU$3,1) &amp; RIGHT(plant_md!CU$3,LEN(plant_md!CU$3)-FIND(" ",plant_md!CU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CU$1,"")</f>
         <v/>
       </c>
       <c r="CV25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CV2),"","_") &amp; UPPER(LEFT(stand_md!CV2,3)) &amp; IF(ISBLANK(stand_md!CV4),"","_") &amp; UPPER(LEFT(stand_md!CV4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CV$3,1) &amp; RIGHT(plant_md!CV$3,LEN(plant_md!CV$3)-FIND(" ",plant_md!CV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CV$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CV$3,1) &amp; RIGHT(plant_md!CV$3,LEN(plant_md!CV$3)-FIND(" ",plant_md!CV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CV$1,"")</f>
         <v/>
       </c>
       <c r="CW25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CW2),"","_") &amp; UPPER(LEFT(stand_md!CW2,3)) &amp; IF(ISBLANK(stand_md!CW4),"","_") &amp; UPPER(LEFT(stand_md!CW4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CW$3,1) &amp; RIGHT(plant_md!CW$3,LEN(plant_md!CW$3)-FIND(" ",plant_md!CW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CW$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CW$3,1) &amp; RIGHT(plant_md!CW$3,LEN(plant_md!CW$3)-FIND(" ",plant_md!CW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CW$1,"")</f>
         <v/>
       </c>
       <c r="CX25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CX2),"","_") &amp; UPPER(LEFT(stand_md!CX2,3)) &amp; IF(ISBLANK(stand_md!CX4),"","_") &amp; UPPER(LEFT(stand_md!CX4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CX$3,1) &amp; RIGHT(plant_md!CX$3,LEN(plant_md!CX$3)-FIND(" ",plant_md!CX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CX$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CX$3,1) &amp; RIGHT(plant_md!CX$3,LEN(plant_md!CX$3)-FIND(" ",plant_md!CX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CX$1,"")</f>
         <v/>
       </c>
       <c r="CY25" s="96" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CY2),"","_") &amp; UPPER(LEFT(stand_md!CY2,3)) &amp; IF(ISBLANK(stand_md!CY4),"","_") &amp; UPPER(LEFT(stand_md!CY4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CY$3,1) &amp; RIGHT(plant_md!CY$3,LEN(plant_md!CY$3)-FIND(" ",plant_md!CY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CY$1,"")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CY$3,1) &amp; RIGHT(plant_md!CY$3,LEN(plant_md!CY$3)-FIND(" ",plant_md!CY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CY$1,"")</f>
         <v/>
       </c>
     </row>
@@ -11034,7 +11034,7 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
@@ -11370,7 +11370,7 @@
   </sheetPr>
   <dimension ref="A1:CW23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -12907,403 +12907,403 @@
         <v>901</v>
       </c>
       <c r="B5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!D$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!D2),"","_") &amp; UPPER(LEFT(stand_md!D2,3)) &amp; IF(ISBLANK(stand_md!D4),"","_") &amp; UPPER(LEFT(stand_md!D4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!D$3,1) &amp; RIGHT(plant_md!D$3,LEN(plant_md!D$3)-FIND(" ",plant_md!D$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!B3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!B3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!D$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!D$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!D$3,1) &amp; RIGHT(plant_md!D$3,LEN(plant_md!D$3)-FIND(" ",plant_md!D$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!B3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!B3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!D$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="C5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!E$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!E2),"","_") &amp; UPPER(LEFT(stand_md!E2,3)) &amp; IF(ISBLANK(stand_md!E4),"","_") &amp; UPPER(LEFT(stand_md!E4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!E$3,1) &amp; RIGHT(plant_md!E$3,LEN(plant_md!E$3)-FIND(" ",plant_md!E$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!C3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!C3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!E$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!E$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!E$3,1) &amp; RIGHT(plant_md!E$3,LEN(plant_md!E$3)-FIND(" ",plant_md!E$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!C3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!C3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!E$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="D5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!F$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!F2),"","_") &amp; UPPER(LEFT(stand_md!F2,3)) &amp; IF(ISBLANK(stand_md!F4),"","_") &amp; UPPER(LEFT(stand_md!F4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!F$3,1) &amp; RIGHT(plant_md!F$3,LEN(plant_md!F$3)-FIND(" ",plant_md!F$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!D3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!D3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!F$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!F$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!F$3,1) &amp; RIGHT(plant_md!F$3,LEN(plant_md!F$3)-FIND(" ",plant_md!F$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!D3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!D3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!F$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="E5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!G$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!G2),"","_") &amp; UPPER(LEFT(stand_md!G2,3)) &amp; IF(ISBLANK(stand_md!G4),"","_") &amp; UPPER(LEFT(stand_md!G4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!G$3,1) &amp; RIGHT(plant_md!G$3,LEN(plant_md!G$3)-FIND(" ",plant_md!G$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!E3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!E3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!G$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!G$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!G$3,1) &amp; RIGHT(plant_md!G$3,LEN(plant_md!G$3)-FIND(" ",plant_md!G$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!E3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!E3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!G$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="F5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!H$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!H2),"","_") &amp; UPPER(LEFT(stand_md!H2,3)) &amp; IF(ISBLANK(stand_md!H4),"","_") &amp; UPPER(LEFT(stand_md!H4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!H$3,1) &amp; RIGHT(plant_md!H$3,LEN(plant_md!H$3)-FIND(" ",plant_md!H$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!F3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!F3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!H$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!H$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!H$3,1) &amp; RIGHT(plant_md!H$3,LEN(plant_md!H$3)-FIND(" ",plant_md!H$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!F3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!F3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!H$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="G5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!I$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!I2),"","_") &amp; UPPER(LEFT(stand_md!I2,3)) &amp; IF(ISBLANK(stand_md!I4),"","_") &amp; UPPER(LEFT(stand_md!I4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!I$3,1) &amp; RIGHT(plant_md!I$3,LEN(plant_md!I$3)-FIND(" ",plant_md!I$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!G3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!G3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!I$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!I$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!I$3,1) &amp; RIGHT(plant_md!I$3,LEN(plant_md!I$3)-FIND(" ",plant_md!I$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!G3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!G3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!I$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="H5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!J$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!J2),"","_") &amp; UPPER(LEFT(stand_md!J2,3)) &amp; IF(ISBLANK(stand_md!J4),"","_") &amp; UPPER(LEFT(stand_md!J4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!J$3,1) &amp; RIGHT(plant_md!J$3,LEN(plant_md!J$3)-FIND(" ",plant_md!J$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!H3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!H3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!J$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!J$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!J$3,1) &amp; RIGHT(plant_md!J$3,LEN(plant_md!J$3)-FIND(" ",plant_md!J$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!H3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!H3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!J$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="I5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!K$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!K2),"","_") &amp; UPPER(LEFT(stand_md!K2,3)) &amp; IF(ISBLANK(stand_md!K4),"","_") &amp; UPPER(LEFT(stand_md!K4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!K$3,1) &amp; RIGHT(plant_md!K$3,LEN(plant_md!K$3)-FIND(" ",plant_md!K$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!I3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!I3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!K$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!K$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!K$3,1) &amp; RIGHT(plant_md!K$3,LEN(plant_md!K$3)-FIND(" ",plant_md!K$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!I3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!I3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!K$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="J5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!L$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!L2),"","_") &amp; UPPER(LEFT(stand_md!L2,3)) &amp; IF(ISBLANK(stand_md!L4),"","_") &amp; UPPER(LEFT(stand_md!L4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!L$3,1) &amp; RIGHT(plant_md!L$3,LEN(plant_md!L$3)-FIND(" ",plant_md!L$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!J3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!J3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!L$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!L$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!L$3,1) &amp; RIGHT(plant_md!L$3,LEN(plant_md!L$3)-FIND(" ",plant_md!L$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!J3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!J3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!L$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="K5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!M$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!M2),"","_") &amp; UPPER(LEFT(stand_md!M2,3)) &amp; IF(ISBLANK(stand_md!M4),"","_") &amp; UPPER(LEFT(stand_md!M4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!M$3,1) &amp; RIGHT(plant_md!M$3,LEN(plant_md!M$3)-FIND(" ",plant_md!M$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!K3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!K3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!M$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!M$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!M$3,1) &amp; RIGHT(plant_md!M$3,LEN(plant_md!M$3)-FIND(" ",plant_md!M$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!K3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!K3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!M$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="L5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!N$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!N2),"","_") &amp; UPPER(LEFT(stand_md!N2,3)) &amp; IF(ISBLANK(stand_md!N4),"","_") &amp; UPPER(LEFT(stand_md!N4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!N$3,1) &amp; RIGHT(plant_md!N$3,LEN(plant_md!N$3)-FIND(" ",plant_md!N$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!L3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!L3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!N$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!N$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!N$3,1) &amp; RIGHT(plant_md!N$3,LEN(plant_md!N$3)-FIND(" ",plant_md!N$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!L3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!L3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!N$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="M5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!O$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!O2),"","_") &amp; UPPER(LEFT(stand_md!O2,3)) &amp; IF(ISBLANK(stand_md!O4),"","_") &amp; UPPER(LEFT(stand_md!O4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!O$3,1) &amp; RIGHT(plant_md!O$3,LEN(plant_md!O$3)-FIND(" ",plant_md!O$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!M3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!M3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!O$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!O$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!O$3,1) &amp; RIGHT(plant_md!O$3,LEN(plant_md!O$3)-FIND(" ",plant_md!O$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!M3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!M3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!O$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="N5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!P$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!P2),"","_") &amp; UPPER(LEFT(stand_md!P2,3)) &amp; IF(ISBLANK(stand_md!P4),"","_") &amp; UPPER(LEFT(stand_md!P4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!P$3,1) &amp; RIGHT(plant_md!P$3,LEN(plant_md!P$3)-FIND(" ",plant_md!P$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!N3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!N3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!P$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!P$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!P$3,1) &amp; RIGHT(plant_md!P$3,LEN(plant_md!P$3)-FIND(" ",plant_md!P$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!N3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!N3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!P$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="O5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!Q$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!Q2),"","_") &amp; UPPER(LEFT(stand_md!Q2,3)) &amp; IF(ISBLANK(stand_md!Q4),"","_") &amp; UPPER(LEFT(stand_md!Q4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Q$3,1) &amp; RIGHT(plant_md!Q$3,LEN(plant_md!Q$3)-FIND(" ",plant_md!Q$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!O3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!O3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Q$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!Q$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Q$3,1) &amp; RIGHT(plant_md!Q$3,LEN(plant_md!Q$3)-FIND(" ",plant_md!Q$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!O3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!O3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Q$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="P5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!R$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!R2),"","_") &amp; UPPER(LEFT(stand_md!R2,3)) &amp; IF(ISBLANK(stand_md!R4),"","_") &amp; UPPER(LEFT(stand_md!R4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!R$3,1) &amp; RIGHT(plant_md!R$3,LEN(plant_md!R$3)-FIND(" ",plant_md!R$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!P3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!P3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!R$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!R$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!R$3,1) &amp; RIGHT(plant_md!R$3,LEN(plant_md!R$3)-FIND(" ",plant_md!R$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!P3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!P3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!R$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="Q5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!S$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!S2),"","_") &amp; UPPER(LEFT(stand_md!S2,3)) &amp; IF(ISBLANK(stand_md!S4),"","_") &amp; UPPER(LEFT(stand_md!S4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!S$3,1) &amp; RIGHT(plant_md!S$3,LEN(plant_md!S$3)-FIND(" ",plant_md!S$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Q3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Q3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!S$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!S$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!S$3,1) &amp; RIGHT(plant_md!S$3,LEN(plant_md!S$3)-FIND(" ",plant_md!S$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Q3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Q3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!S$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="R5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!T$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!T2),"","_") &amp; UPPER(LEFT(stand_md!T2,3)) &amp; IF(ISBLANK(stand_md!T4),"","_") &amp; UPPER(LEFT(stand_md!T4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!T$3,1) &amp; RIGHT(plant_md!T$3,LEN(plant_md!T$3)-FIND(" ",plant_md!T$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!R3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!R3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!T$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!T$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!T$3,1) &amp; RIGHT(plant_md!T$3,LEN(plant_md!T$3)-FIND(" ",plant_md!T$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!R3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!R3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!T$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="S5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!U$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!U2),"","_") &amp; UPPER(LEFT(stand_md!U2,3)) &amp; IF(ISBLANK(stand_md!U4),"","_") &amp; UPPER(LEFT(stand_md!U4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!U$3,1) &amp; RIGHT(plant_md!U$3,LEN(plant_md!U$3)-FIND(" ",plant_md!U$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!S3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!S3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!U$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!U$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!U$3,1) &amp; RIGHT(plant_md!U$3,LEN(plant_md!U$3)-FIND(" ",plant_md!U$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!S3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!S3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!U$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="T5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!V$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!V2),"","_") &amp; UPPER(LEFT(stand_md!V2,3)) &amp; IF(ISBLANK(stand_md!V4),"","_") &amp; UPPER(LEFT(stand_md!V4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!V$3,1) &amp; RIGHT(plant_md!V$3,LEN(plant_md!V$3)-FIND(" ",plant_md!V$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!T3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!T3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!V$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!V$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!V$3,1) &amp; RIGHT(plant_md!V$3,LEN(plant_md!V$3)-FIND(" ",plant_md!V$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!T3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!T3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!V$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="U5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!W$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!W2),"","_") &amp; UPPER(LEFT(stand_md!W2,3)) &amp; IF(ISBLANK(stand_md!W4),"","_") &amp; UPPER(LEFT(stand_md!W4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!W$3,1) &amp; RIGHT(plant_md!W$3,LEN(plant_md!W$3)-FIND(" ",plant_md!W$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!U3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!U3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!W$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!W$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!W$3,1) &amp; RIGHT(plant_md!W$3,LEN(plant_md!W$3)-FIND(" ",plant_md!W$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!U3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!U3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!W$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="V5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!X$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!X2),"","_") &amp; UPPER(LEFT(stand_md!X2,3)) &amp; IF(ISBLANK(stand_md!X4),"","_") &amp; UPPER(LEFT(stand_md!X4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!X$3,1) &amp; RIGHT(plant_md!X$3,LEN(plant_md!X$3)-FIND(" ",plant_md!X$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!V3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!V3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!X$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!X$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!X$3,1) &amp; RIGHT(plant_md!X$3,LEN(plant_md!X$3)-FIND(" ",plant_md!X$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!V3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!V3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!X$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="W5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!Y$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!Y2),"","_") &amp; UPPER(LEFT(stand_md!Y2,3)) &amp; IF(ISBLANK(stand_md!Y4),"","_") &amp; UPPER(LEFT(stand_md!Y4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Y$3,1) &amp; RIGHT(plant_md!Y$3,LEN(plant_md!Y$3)-FIND(" ",plant_md!Y$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!W3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!W3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Y$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!Y$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Y$3,1) &amp; RIGHT(plant_md!Y$3,LEN(plant_md!Y$3)-FIND(" ",plant_md!Y$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!W3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!W3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Y$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="X5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!Z$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!Z2),"","_") &amp; UPPER(LEFT(stand_md!Z2,3)) &amp; IF(ISBLANK(stand_md!Z4),"","_") &amp; UPPER(LEFT(stand_md!Z4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Z$3,1) &amp; RIGHT(plant_md!Z$3,LEN(plant_md!Z$3)-FIND(" ",plant_md!Z$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!X3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!X3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Z$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!Z$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!Z$3,1) &amp; RIGHT(plant_md!Z$3,LEN(plant_md!Z$3)-FIND(" ",plant_md!Z$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!X3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!X3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!Z$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="Y5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AA2),"","_") &amp; UPPER(LEFT(stand_md!AA2,3)) &amp; IF(ISBLANK(stand_md!AA4),"","_") &amp; UPPER(LEFT(stand_md!AA4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AA$3,1) &amp; RIGHT(plant_md!AA$3,LEN(plant_md!AA$3)-FIND(" ",plant_md!AA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Y3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Y3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AA$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AA$3,1) &amp; RIGHT(plant_md!AA$3,LEN(plant_md!AA$3)-FIND(" ",plant_md!AA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Y3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Y3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AA$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="Z5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AB2),"","_") &amp; UPPER(LEFT(stand_md!AB2,3)) &amp; IF(ISBLANK(stand_md!AB4),"","_") &amp; UPPER(LEFT(stand_md!AB4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AB$3,1) &amp; RIGHT(plant_md!AB$3,LEN(plant_md!AB$3)-FIND(" ",plant_md!AB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Z3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Z3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AB$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AB$3,1) &amp; RIGHT(plant_md!AB$3,LEN(plant_md!AB$3)-FIND(" ",plant_md!AB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!Z3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!Z3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AB$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AA5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AC2),"","_") &amp; UPPER(LEFT(stand_md!AC2,3)) &amp; IF(ISBLANK(stand_md!AC4),"","_") &amp; UPPER(LEFT(stand_md!AC4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AC$3,1) &amp; RIGHT(plant_md!AC$3,LEN(plant_md!AC$3)-FIND(" ",plant_md!AC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AC$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AC$3,1) &amp; RIGHT(plant_md!AC$3,LEN(plant_md!AC$3)-FIND(" ",plant_md!AC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AC$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AB5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AD2),"","_") &amp; UPPER(LEFT(stand_md!AD2,3)) &amp; IF(ISBLANK(stand_md!AD4),"","_") &amp; UPPER(LEFT(stand_md!AD4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AD$3,1) &amp; RIGHT(plant_md!AD$3,LEN(plant_md!AD$3)-FIND(" ",plant_md!AD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AD$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AD$3,1) &amp; RIGHT(plant_md!AD$3,LEN(plant_md!AD$3)-FIND(" ",plant_md!AD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AD$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AC5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AE2),"","_") &amp; UPPER(LEFT(stand_md!AE2,3)) &amp; IF(ISBLANK(stand_md!AE4),"","_") &amp; UPPER(LEFT(stand_md!AE4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AE$3,1) &amp; RIGHT(plant_md!AE$3,LEN(plant_md!AE$3)-FIND(" ",plant_md!AE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AE$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AE$3,1) &amp; RIGHT(plant_md!AE$3,LEN(plant_md!AE$3)-FIND(" ",plant_md!AE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AE$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AD5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AF2),"","_") &amp; UPPER(LEFT(stand_md!AF2,3)) &amp; IF(ISBLANK(stand_md!AF4),"","_") &amp; UPPER(LEFT(stand_md!AF4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AF$3,1) &amp; RIGHT(plant_md!AF$3,LEN(plant_md!AF$3)-FIND(" ",plant_md!AF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AF$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AF$3,1) &amp; RIGHT(plant_md!AF$3,LEN(plant_md!AF$3)-FIND(" ",plant_md!AF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AF$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AE5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AG2),"","_") &amp; UPPER(LEFT(stand_md!AG2,3)) &amp; IF(ISBLANK(stand_md!AG4),"","_") &amp; UPPER(LEFT(stand_md!AG4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AG$3,1) &amp; RIGHT(plant_md!AG$3,LEN(plant_md!AG$3)-FIND(" ",plant_md!AG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AG$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AG$3,1) &amp; RIGHT(plant_md!AG$3,LEN(plant_md!AG$3)-FIND(" ",plant_md!AG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AG$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AF5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AH2),"","_") &amp; UPPER(LEFT(stand_md!AH2,3)) &amp; IF(ISBLANK(stand_md!AH4),"","_") &amp; UPPER(LEFT(stand_md!AH4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AH$3,1) &amp; RIGHT(plant_md!AH$3,LEN(plant_md!AH$3)-FIND(" ",plant_md!AH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AH$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AH$3,1) &amp; RIGHT(plant_md!AH$3,LEN(plant_md!AH$3)-FIND(" ",plant_md!AH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AH$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AG5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AI2),"","_") &amp; UPPER(LEFT(stand_md!AI2,3)) &amp; IF(ISBLANK(stand_md!AI4),"","_") &amp; UPPER(LEFT(stand_md!AI4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AI$3,1) &amp; RIGHT(plant_md!AI$3,LEN(plant_md!AI$3)-FIND(" ",plant_md!AI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AI$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AI$3,1) &amp; RIGHT(plant_md!AI$3,LEN(plant_md!AI$3)-FIND(" ",plant_md!AI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AI$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AH5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AJ2),"","_") &amp; UPPER(LEFT(stand_md!AJ2,3)) &amp; IF(ISBLANK(stand_md!AJ4),"","_") &amp; UPPER(LEFT(stand_md!AJ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AJ$3,1) &amp; RIGHT(plant_md!AJ$3,LEN(plant_md!AJ$3)-FIND(" ",plant_md!AJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AJ$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AJ$3,1) &amp; RIGHT(plant_md!AJ$3,LEN(plant_md!AJ$3)-FIND(" ",plant_md!AJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AJ$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AI5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AK2),"","_") &amp; UPPER(LEFT(stand_md!AK2,3)) &amp; IF(ISBLANK(stand_md!AK4),"","_") &amp; UPPER(LEFT(stand_md!AK4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AK$3,1) &amp; RIGHT(plant_md!AK$3,LEN(plant_md!AK$3)-FIND(" ",plant_md!AK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AK$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AK$3,1) &amp; RIGHT(plant_md!AK$3,LEN(plant_md!AK$3)-FIND(" ",plant_md!AK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AK$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AJ5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AL2),"","_") &amp; UPPER(LEFT(stand_md!AL2,3)) &amp; IF(ISBLANK(stand_md!AL4),"","_") &amp; UPPER(LEFT(stand_md!AL4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AL$3,1) &amp; RIGHT(plant_md!AL$3,LEN(plant_md!AL$3)-FIND(" ",plant_md!AL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AL$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AL$3,1) &amp; RIGHT(plant_md!AL$3,LEN(plant_md!AL$3)-FIND(" ",plant_md!AL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AL$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AK5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AM2),"","_") &amp; UPPER(LEFT(stand_md!AM2,3)) &amp; IF(ISBLANK(stand_md!AM4),"","_") &amp; UPPER(LEFT(stand_md!AM4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AM$3,1) &amp; RIGHT(plant_md!AM$3,LEN(plant_md!AM$3)-FIND(" ",plant_md!AM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AM$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AM$3,1) &amp; RIGHT(plant_md!AM$3,LEN(plant_md!AM$3)-FIND(" ",plant_md!AM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AM$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AL5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AN2),"","_") &amp; UPPER(LEFT(stand_md!AN2,3)) &amp; IF(ISBLANK(stand_md!AN4),"","_") &amp; UPPER(LEFT(stand_md!AN4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AN$3,1) &amp; RIGHT(plant_md!AN$3,LEN(plant_md!AN$3)-FIND(" ",plant_md!AN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AN$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AN$3,1) &amp; RIGHT(plant_md!AN$3,LEN(plant_md!AN$3)-FIND(" ",plant_md!AN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AN$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AM5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AO2),"","_") &amp; UPPER(LEFT(stand_md!AO2,3)) &amp; IF(ISBLANK(stand_md!AO4),"","_") &amp; UPPER(LEFT(stand_md!AO4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AO$3,1) &amp; RIGHT(plant_md!AO$3,LEN(plant_md!AO$3)-FIND(" ",plant_md!AO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AO$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AO$3,1) &amp; RIGHT(plant_md!AO$3,LEN(plant_md!AO$3)-FIND(" ",plant_md!AO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AO$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AN5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AP2),"","_") &amp; UPPER(LEFT(stand_md!AP2,3)) &amp; IF(ISBLANK(stand_md!AP4),"","_") &amp; UPPER(LEFT(stand_md!AP4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AP$3,1) &amp; RIGHT(plant_md!AP$3,LEN(plant_md!AP$3)-FIND(" ",plant_md!AP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AP$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AP$3,1) &amp; RIGHT(plant_md!AP$3,LEN(plant_md!AP$3)-FIND(" ",plant_md!AP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AP$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AO5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AQ2),"","_") &amp; UPPER(LEFT(stand_md!AQ2,3)) &amp; IF(ISBLANK(stand_md!AQ4),"","_") &amp; UPPER(LEFT(stand_md!AQ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AQ$3,1) &amp; RIGHT(plant_md!AQ$3,LEN(plant_md!AQ$3)-FIND(" ",plant_md!AQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AQ$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AQ$3,1) &amp; RIGHT(plant_md!AQ$3,LEN(plant_md!AQ$3)-FIND(" ",plant_md!AQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AQ$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AP5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AR2),"","_") &amp; UPPER(LEFT(stand_md!AR2,3)) &amp; IF(ISBLANK(stand_md!AR4),"","_") &amp; UPPER(LEFT(stand_md!AR4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AR$3,1) &amp; RIGHT(plant_md!AR$3,LEN(plant_md!AR$3)-FIND(" ",plant_md!AR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AR$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AR$3,1) &amp; RIGHT(plant_md!AR$3,LEN(plant_md!AR$3)-FIND(" ",plant_md!AR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AR$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AQ5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AS2),"","_") &amp; UPPER(LEFT(stand_md!AS2,3)) &amp; IF(ISBLANK(stand_md!AS4),"","_") &amp; UPPER(LEFT(stand_md!AS4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AS$3,1) &amp; RIGHT(plant_md!AS$3,LEN(plant_md!AS$3)-FIND(" ",plant_md!AS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AS$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AS$3,1) &amp; RIGHT(plant_md!AS$3,LEN(plant_md!AS$3)-FIND(" ",plant_md!AS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AS$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AR5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AT2),"","_") &amp; UPPER(LEFT(stand_md!AT2,3)) &amp; IF(ISBLANK(stand_md!AT4),"","_") &amp; UPPER(LEFT(stand_md!AT4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AT$3,1) &amp; RIGHT(plant_md!AT$3,LEN(plant_md!AT$3)-FIND(" ",plant_md!AT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AT$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AT$3,1) &amp; RIGHT(plant_md!AT$3,LEN(plant_md!AT$3)-FIND(" ",plant_md!AT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AT$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AS5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AU2),"","_") &amp; UPPER(LEFT(stand_md!AU2,3)) &amp; IF(ISBLANK(stand_md!AU4),"","_") &amp; UPPER(LEFT(stand_md!AU4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AU$3,1) &amp; RIGHT(plant_md!AU$3,LEN(plant_md!AU$3)-FIND(" ",plant_md!AU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AU$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AU$3,1) &amp; RIGHT(plant_md!AU$3,LEN(plant_md!AU$3)-FIND(" ",plant_md!AU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AU$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AT5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AV2),"","_") &amp; UPPER(LEFT(stand_md!AV2,3)) &amp; IF(ISBLANK(stand_md!AV4),"","_") &amp; UPPER(LEFT(stand_md!AV4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AV$3,1) &amp; RIGHT(plant_md!AV$3,LEN(plant_md!AV$3)-FIND(" ",plant_md!AV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AV$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AV$3,1) &amp; RIGHT(plant_md!AV$3,LEN(plant_md!AV$3)-FIND(" ",plant_md!AV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AV$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AU5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AW2),"","_") &amp; UPPER(LEFT(stand_md!AW2,3)) &amp; IF(ISBLANK(stand_md!AW4),"","_") &amp; UPPER(LEFT(stand_md!AW4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AW$3,1) &amp; RIGHT(plant_md!AW$3,LEN(plant_md!AW$3)-FIND(" ",plant_md!AW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AW$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AW$3,1) &amp; RIGHT(plant_md!AW$3,LEN(plant_md!AW$3)-FIND(" ",plant_md!AW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AW$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AV5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AX2),"","_") &amp; UPPER(LEFT(stand_md!AX2,3)) &amp; IF(ISBLANK(stand_md!AX4),"","_") &amp; UPPER(LEFT(stand_md!AX4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AX$3,1) &amp; RIGHT(plant_md!AX$3,LEN(plant_md!AX$3)-FIND(" ",plant_md!AX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AX$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AX$3,1) &amp; RIGHT(plant_md!AX$3,LEN(plant_md!AX$3)-FIND(" ",plant_md!AX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AX$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AW5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AY2),"","_") &amp; UPPER(LEFT(stand_md!AY2,3)) &amp; IF(ISBLANK(stand_md!AY4),"","_") &amp; UPPER(LEFT(stand_md!AY4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AY$3,1) &amp; RIGHT(plant_md!AY$3,LEN(plant_md!AY$3)-FIND(" ",plant_md!AY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AY$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AY$3,1) &amp; RIGHT(plant_md!AY$3,LEN(plant_md!AY$3)-FIND(" ",plant_md!AY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AY$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AX5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!AZ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!AZ2),"","_") &amp; UPPER(LEFT(stand_md!AZ2,3)) &amp; IF(ISBLANK(stand_md!AZ4),"","_") &amp; UPPER(LEFT(stand_md!AZ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AZ$3,1) &amp; RIGHT(plant_md!AZ$3,LEN(plant_md!AZ$3)-FIND(" ",plant_md!AZ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AZ$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!AZ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!AZ$3,1) &amp; RIGHT(plant_md!AZ$3,LEN(plant_md!AZ$3)-FIND(" ",plant_md!AZ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!AZ$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AY5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BA2),"","_") &amp; UPPER(LEFT(stand_md!BA2,3)) &amp; IF(ISBLANK(stand_md!BA4),"","_") &amp; UPPER(LEFT(stand_md!BA4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BA$3,1) &amp; RIGHT(plant_md!BA$3,LEN(plant_md!BA$3)-FIND(" ",plant_md!BA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BA$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BA$3,1) &amp; RIGHT(plant_md!BA$3,LEN(plant_md!BA$3)-FIND(" ",plant_md!BA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BA$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="AZ5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BB2),"","_") &amp; UPPER(LEFT(stand_md!BB2,3)) &amp; IF(ISBLANK(stand_md!BB4),"","_") &amp; UPPER(LEFT(stand_md!BB4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BB$3,1) &amp; RIGHT(plant_md!BB$3,LEN(plant_md!BB$3)-FIND(" ",plant_md!BB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BB$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BB$3,1) &amp; RIGHT(plant_md!BB$3,LEN(plant_md!BB$3)-FIND(" ",plant_md!BB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!AZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!AZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BB$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BA5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BC2),"","_") &amp; UPPER(LEFT(stand_md!BC2,3)) &amp; IF(ISBLANK(stand_md!BC4),"","_") &amp; UPPER(LEFT(stand_md!BC4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BC$3,1) &amp; RIGHT(plant_md!BC$3,LEN(plant_md!BC$3)-FIND(" ",plant_md!BC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BC$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BC$3,1) &amp; RIGHT(plant_md!BC$3,LEN(plant_md!BC$3)-FIND(" ",plant_md!BC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BC$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BB5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BD2),"","_") &amp; UPPER(LEFT(stand_md!BD2,3)) &amp; IF(ISBLANK(stand_md!BD4),"","_") &amp; UPPER(LEFT(stand_md!BD4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BD$3,1) &amp; RIGHT(plant_md!BD$3,LEN(plant_md!BD$3)-FIND(" ",plant_md!BD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BD$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BD$3,1) &amp; RIGHT(plant_md!BD$3,LEN(plant_md!BD$3)-FIND(" ",plant_md!BD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BD$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BC5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BE2),"","_") &amp; UPPER(LEFT(stand_md!BE2,3)) &amp; IF(ISBLANK(stand_md!BE4),"","_") &amp; UPPER(LEFT(stand_md!BE4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BE$3,1) &amp; RIGHT(plant_md!BE$3,LEN(plant_md!BE$3)-FIND(" ",plant_md!BE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BE$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BE$3,1) &amp; RIGHT(plant_md!BE$3,LEN(plant_md!BE$3)-FIND(" ",plant_md!BE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BE$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BD5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BF2),"","_") &amp; UPPER(LEFT(stand_md!BF2,3)) &amp; IF(ISBLANK(stand_md!BF4),"","_") &amp; UPPER(LEFT(stand_md!BF4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BF$3,1) &amp; RIGHT(plant_md!BF$3,LEN(plant_md!BF$3)-FIND(" ",plant_md!BF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BF$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BF$3,1) &amp; RIGHT(plant_md!BF$3,LEN(plant_md!BF$3)-FIND(" ",plant_md!BF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BF$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BE5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BG2),"","_") &amp; UPPER(LEFT(stand_md!BG2,3)) &amp; IF(ISBLANK(stand_md!BG4),"","_") &amp; UPPER(LEFT(stand_md!BG4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BG$3,1) &amp; RIGHT(plant_md!BG$3,LEN(plant_md!BG$3)-FIND(" ",plant_md!BG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BG$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BG$3,1) &amp; RIGHT(plant_md!BG$3,LEN(plant_md!BG$3)-FIND(" ",plant_md!BG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BG$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BF5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BH2),"","_") &amp; UPPER(LEFT(stand_md!BH2,3)) &amp; IF(ISBLANK(stand_md!BH4),"","_") &amp; UPPER(LEFT(stand_md!BH4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BH$3,1) &amp; RIGHT(plant_md!BH$3,LEN(plant_md!BH$3)-FIND(" ",plant_md!BH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BH$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BH$3,1) &amp; RIGHT(plant_md!BH$3,LEN(plant_md!BH$3)-FIND(" ",plant_md!BH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BH$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BG5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BI2),"","_") &amp; UPPER(LEFT(stand_md!BI2,3)) &amp; IF(ISBLANK(stand_md!BI4),"","_") &amp; UPPER(LEFT(stand_md!BI4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BI$3,1) &amp; RIGHT(plant_md!BI$3,LEN(plant_md!BI$3)-FIND(" ",plant_md!BI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BI$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BI$3,1) &amp; RIGHT(plant_md!BI$3,LEN(plant_md!BI$3)-FIND(" ",plant_md!BI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BI$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BH5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BJ2),"","_") &amp; UPPER(LEFT(stand_md!BJ2,3)) &amp; IF(ISBLANK(stand_md!BJ4),"","_") &amp; UPPER(LEFT(stand_md!BJ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BJ$3,1) &amp; RIGHT(plant_md!BJ$3,LEN(plant_md!BJ$3)-FIND(" ",plant_md!BJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BJ$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BJ$3,1) &amp; RIGHT(plant_md!BJ$3,LEN(plant_md!BJ$3)-FIND(" ",plant_md!BJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BJ$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BI5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BK2),"","_") &amp; UPPER(LEFT(stand_md!BK2,3)) &amp; IF(ISBLANK(stand_md!BK4),"","_") &amp; UPPER(LEFT(stand_md!BK4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BK$3,1) &amp; RIGHT(plant_md!BK$3,LEN(plant_md!BK$3)-FIND(" ",plant_md!BK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BK$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BK$3,1) &amp; RIGHT(plant_md!BK$3,LEN(plant_md!BK$3)-FIND(" ",plant_md!BK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BK$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BJ5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BL2),"","_") &amp; UPPER(LEFT(stand_md!BL2,3)) &amp; IF(ISBLANK(stand_md!BL4),"","_") &amp; UPPER(LEFT(stand_md!BL4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BL$3,1) &amp; RIGHT(plant_md!BL$3,LEN(plant_md!BL$3)-FIND(" ",plant_md!BL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BL$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BL$3,1) &amp; RIGHT(plant_md!BL$3,LEN(plant_md!BL$3)-FIND(" ",plant_md!BL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BL$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BK5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BM2),"","_") &amp; UPPER(LEFT(stand_md!BM2,3)) &amp; IF(ISBLANK(stand_md!BM4),"","_") &amp; UPPER(LEFT(stand_md!BM4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BM$3,1) &amp; RIGHT(plant_md!BM$3,LEN(plant_md!BM$3)-FIND(" ",plant_md!BM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BM$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BM$3,1) &amp; RIGHT(plant_md!BM$3,LEN(plant_md!BM$3)-FIND(" ",plant_md!BM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BM$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BL5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BN2),"","_") &amp; UPPER(LEFT(stand_md!BN2,3)) &amp; IF(ISBLANK(stand_md!BN4),"","_") &amp; UPPER(LEFT(stand_md!BN4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BN$3,1) &amp; RIGHT(plant_md!BN$3,LEN(plant_md!BN$3)-FIND(" ",plant_md!BN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BN$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BN$3,1) &amp; RIGHT(plant_md!BN$3,LEN(plant_md!BN$3)-FIND(" ",plant_md!BN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BN$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BM5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BO2),"","_") &amp; UPPER(LEFT(stand_md!BO2,3)) &amp; IF(ISBLANK(stand_md!BO4),"","_") &amp; UPPER(LEFT(stand_md!BO4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BO$3,1) &amp; RIGHT(plant_md!BO$3,LEN(plant_md!BO$3)-FIND(" ",plant_md!BO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BO$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BO$3,1) &amp; RIGHT(plant_md!BO$3,LEN(plant_md!BO$3)-FIND(" ",plant_md!BO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BO$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BN5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BP2),"","_") &amp; UPPER(LEFT(stand_md!BP2,3)) &amp; IF(ISBLANK(stand_md!BP4),"","_") &amp; UPPER(LEFT(stand_md!BP4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BP$3,1) &amp; RIGHT(plant_md!BP$3,LEN(plant_md!BP$3)-FIND(" ",plant_md!BP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BP$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BP$3,1) &amp; RIGHT(plant_md!BP$3,LEN(plant_md!BP$3)-FIND(" ",plant_md!BP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BP$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BO5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BQ2),"","_") &amp; UPPER(LEFT(stand_md!BQ2,3)) &amp; IF(ISBLANK(stand_md!BQ4),"","_") &amp; UPPER(LEFT(stand_md!BQ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BQ$3,1) &amp; RIGHT(plant_md!BQ$3,LEN(plant_md!BQ$3)-FIND(" ",plant_md!BQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BQ$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BQ$3,1) &amp; RIGHT(plant_md!BQ$3,LEN(plant_md!BQ$3)-FIND(" ",plant_md!BQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BQ$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BP5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BR2),"","_") &amp; UPPER(LEFT(stand_md!BR2,3)) &amp; IF(ISBLANK(stand_md!BR4),"","_") &amp; UPPER(LEFT(stand_md!BR4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BR$3,1) &amp; RIGHT(plant_md!BR$3,LEN(plant_md!BR$3)-FIND(" ",plant_md!BR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BR$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BR$3,1) &amp; RIGHT(plant_md!BR$3,LEN(plant_md!BR$3)-FIND(" ",plant_md!BR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BR$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BQ5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BS2),"","_") &amp; UPPER(LEFT(stand_md!BS2,3)) &amp; IF(ISBLANK(stand_md!BS4),"","_") &amp; UPPER(LEFT(stand_md!BS4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BS$3,1) &amp; RIGHT(plant_md!BS$3,LEN(plant_md!BS$3)-FIND(" ",plant_md!BS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BS$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BS$3,1) &amp; RIGHT(plant_md!BS$3,LEN(plant_md!BS$3)-FIND(" ",plant_md!BS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BS$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BR5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BT2),"","_") &amp; UPPER(LEFT(stand_md!BT2,3)) &amp; IF(ISBLANK(stand_md!BT4),"","_") &amp; UPPER(LEFT(stand_md!BT4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BT$3,1) &amp; RIGHT(plant_md!BT$3,LEN(plant_md!BT$3)-FIND(" ",plant_md!BT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BT$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BT$3,1) &amp; RIGHT(plant_md!BT$3,LEN(plant_md!BT$3)-FIND(" ",plant_md!BT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BT$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BS5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BU2),"","_") &amp; UPPER(LEFT(stand_md!BU2,3)) &amp; IF(ISBLANK(stand_md!BU4),"","_") &amp; UPPER(LEFT(stand_md!BU4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BU$3,1) &amp; RIGHT(plant_md!BU$3,LEN(plant_md!BU$3)-FIND(" ",plant_md!BU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BU$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BU$3,1) &amp; RIGHT(plant_md!BU$3,LEN(plant_md!BU$3)-FIND(" ",plant_md!BU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BU$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BT5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BV2),"","_") &amp; UPPER(LEFT(stand_md!BV2,3)) &amp; IF(ISBLANK(stand_md!BV4),"","_") &amp; UPPER(LEFT(stand_md!BV4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BV$3,1) &amp; RIGHT(plant_md!BV$3,LEN(plant_md!BV$3)-FIND(" ",plant_md!BV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BV$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BV$3,1) &amp; RIGHT(plant_md!BV$3,LEN(plant_md!BV$3)-FIND(" ",plant_md!BV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BV$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BU5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BW2),"","_") &amp; UPPER(LEFT(stand_md!BW2,3)) &amp; IF(ISBLANK(stand_md!BW4),"","_") &amp; UPPER(LEFT(stand_md!BW4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BW$3,1) &amp; RIGHT(plant_md!BW$3,LEN(plant_md!BW$3)-FIND(" ",plant_md!BW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BW$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BW$3,1) &amp; RIGHT(plant_md!BW$3,LEN(plant_md!BW$3)-FIND(" ",plant_md!BW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BW$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BV5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BX2),"","_") &amp; UPPER(LEFT(stand_md!BX2,3)) &amp; IF(ISBLANK(stand_md!BX4),"","_") &amp; UPPER(LEFT(stand_md!BX4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BX$3,1) &amp; RIGHT(plant_md!BX$3,LEN(plant_md!BX$3)-FIND(" ",plant_md!BX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BX$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BX$3,1) &amp; RIGHT(plant_md!BX$3,LEN(plant_md!BX$3)-FIND(" ",plant_md!BX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BX$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BW5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BY2),"","_") &amp; UPPER(LEFT(stand_md!BY2,3)) &amp; IF(ISBLANK(stand_md!BY4),"","_") &amp; UPPER(LEFT(stand_md!BY4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BY$3,1) &amp; RIGHT(plant_md!BY$3,LEN(plant_md!BY$3)-FIND(" ",plant_md!BY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BY$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BY$3,1) &amp; RIGHT(plant_md!BY$3,LEN(plant_md!BY$3)-FIND(" ",plant_md!BY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BY$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BX5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!BZ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!BZ2),"","_") &amp; UPPER(LEFT(stand_md!BZ2,3)) &amp; IF(ISBLANK(stand_md!BZ4),"","_") &amp; UPPER(LEFT(stand_md!BZ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BZ$3,1) &amp; RIGHT(plant_md!BZ$3,LEN(plant_md!BZ$3)-FIND(" ",plant_md!BZ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BZ$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!BZ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!BZ$3,1) &amp; RIGHT(plant_md!BZ$3,LEN(plant_md!BZ$3)-FIND(" ",plant_md!BZ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BX3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!BZ$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BY5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CA2),"","_") &amp; UPPER(LEFT(stand_md!CA2,3)) &amp; IF(ISBLANK(stand_md!CA4),"","_") &amp; UPPER(LEFT(stand_md!CA4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CA$3,1) &amp; RIGHT(plant_md!CA$3,LEN(plant_md!CA$3)-FIND(" ",plant_md!CA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CA$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CA$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CA$3,1) &amp; RIGHT(plant_md!CA$3,LEN(plant_md!CA$3)-FIND(" ",plant_md!CA$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BY3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CA$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="BZ5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CB2),"","_") &amp; UPPER(LEFT(stand_md!CB2,3)) &amp; IF(ISBLANK(stand_md!CB4),"","_") &amp; UPPER(LEFT(stand_md!CB4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CB$3,1) &amp; RIGHT(plant_md!CB$3,LEN(plant_md!CB$3)-FIND(" ",plant_md!CB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CB$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CB$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CB$3,1) &amp; RIGHT(plant_md!CB$3,LEN(plant_md!CB$3)-FIND(" ",plant_md!CB$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!BZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!BZ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CB$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CA5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CC2),"","_") &amp; UPPER(LEFT(stand_md!CC2,3)) &amp; IF(ISBLANK(stand_md!CC4),"","_") &amp; UPPER(LEFT(stand_md!CC4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CC$3,1) &amp; RIGHT(plant_md!CC$3,LEN(plant_md!CC$3)-FIND(" ",plant_md!CC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CC$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CC$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CC$3,1) &amp; RIGHT(plant_md!CC$3,LEN(plant_md!CC$3)-FIND(" ",plant_md!CC$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CA3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CC$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CB5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CD2),"","_") &amp; UPPER(LEFT(stand_md!CD2,3)) &amp; IF(ISBLANK(stand_md!CD4),"","_") &amp; UPPER(LEFT(stand_md!CD4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CD$3,1) &amp; RIGHT(plant_md!CD$3,LEN(plant_md!CD$3)-FIND(" ",plant_md!CD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CD$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CD$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CD$3,1) &amp; RIGHT(plant_md!CD$3,LEN(plant_md!CD$3)-FIND(" ",plant_md!CD$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CB3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CD$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CC5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CE2),"","_") &amp; UPPER(LEFT(stand_md!CE2,3)) &amp; IF(ISBLANK(stand_md!CE4),"","_") &amp; UPPER(LEFT(stand_md!CE4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CE$3,1) &amp; RIGHT(plant_md!CE$3,LEN(plant_md!CE$3)-FIND(" ",plant_md!CE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CE$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CE$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CE$3,1) &amp; RIGHT(plant_md!CE$3,LEN(plant_md!CE$3)-FIND(" ",plant_md!CE$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CC3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CE$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CD5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CF2),"","_") &amp; UPPER(LEFT(stand_md!CF2,3)) &amp; IF(ISBLANK(stand_md!CF4),"","_") &amp; UPPER(LEFT(stand_md!CF4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CF$3,1) &amp; RIGHT(plant_md!CF$3,LEN(plant_md!CF$3)-FIND(" ",plant_md!CF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CF$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CF$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CF$3,1) &amp; RIGHT(plant_md!CF$3,LEN(plant_md!CF$3)-FIND(" ",plant_md!CF$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CD3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CF$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CE5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CG2),"","_") &amp; UPPER(LEFT(stand_md!CG2,3)) &amp; IF(ISBLANK(stand_md!CG4),"","_") &amp; UPPER(LEFT(stand_md!CG4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CG$3,1) &amp; RIGHT(plant_md!CG$3,LEN(plant_md!CG$3)-FIND(" ",plant_md!CG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CG$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CG$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CG$3,1) &amp; RIGHT(plant_md!CG$3,LEN(plant_md!CG$3)-FIND(" ",plant_md!CG$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CE3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CG$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CF5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CH2),"","_") &amp; UPPER(LEFT(stand_md!CH2,3)) &amp; IF(ISBLANK(stand_md!CH4),"","_") &amp; UPPER(LEFT(stand_md!CH4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CH$3,1) &amp; RIGHT(plant_md!CH$3,LEN(plant_md!CH$3)-FIND(" ",plant_md!CH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CH$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CH$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CH$3,1) &amp; RIGHT(plant_md!CH$3,LEN(plant_md!CH$3)-FIND(" ",plant_md!CH$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CF3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CH$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CG5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CI2),"","_") &amp; UPPER(LEFT(stand_md!CI2,3)) &amp; IF(ISBLANK(stand_md!CI4),"","_") &amp; UPPER(LEFT(stand_md!CI4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CI$3,1) &amp; RIGHT(plant_md!CI$3,LEN(plant_md!CI$3)-FIND(" ",plant_md!CI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CI$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CI$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CI$3,1) &amp; RIGHT(plant_md!CI$3,LEN(plant_md!CI$3)-FIND(" ",plant_md!CI$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CG3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CI$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CH5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CJ2),"","_") &amp; UPPER(LEFT(stand_md!CJ2,3)) &amp; IF(ISBLANK(stand_md!CJ4),"","_") &amp; UPPER(LEFT(stand_md!CJ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CJ$3,1) &amp; RIGHT(plant_md!CJ$3,LEN(plant_md!CJ$3)-FIND(" ",plant_md!CJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CJ$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CJ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CJ$3,1) &amp; RIGHT(plant_md!CJ$3,LEN(plant_md!CJ$3)-FIND(" ",plant_md!CJ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CH3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CJ$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CI5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CK2),"","_") &amp; UPPER(LEFT(stand_md!CK2,3)) &amp; IF(ISBLANK(stand_md!CK4),"","_") &amp; UPPER(LEFT(stand_md!CK4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CK$3,1) &amp; RIGHT(plant_md!CK$3,LEN(plant_md!CK$3)-FIND(" ",plant_md!CK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CK$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CK$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CK$3,1) &amp; RIGHT(plant_md!CK$3,LEN(plant_md!CK$3)-FIND(" ",plant_md!CK$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CI3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CK$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CJ5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CL2),"","_") &amp; UPPER(LEFT(stand_md!CL2,3)) &amp; IF(ISBLANK(stand_md!CL4),"","_") &amp; UPPER(LEFT(stand_md!CL4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CL$3,1) &amp; RIGHT(plant_md!CL$3,LEN(plant_md!CL$3)-FIND(" ",plant_md!CL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CL$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CL$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CL$3,1) &amp; RIGHT(plant_md!CL$3,LEN(plant_md!CL$3)-FIND(" ",plant_md!CL$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CJ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CL$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CK5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CM2),"","_") &amp; UPPER(LEFT(stand_md!CM2,3)) &amp; IF(ISBLANK(stand_md!CM4),"","_") &amp; UPPER(LEFT(stand_md!CM4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CM$3,1) &amp; RIGHT(plant_md!CM$3,LEN(plant_md!CM$3)-FIND(" ",plant_md!CM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CM$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CM$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CM$3,1) &amp; RIGHT(plant_md!CM$3,LEN(plant_md!CM$3)-FIND(" ",plant_md!CM$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CK3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CM$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CL5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CN2),"","_") &amp; UPPER(LEFT(stand_md!CN2,3)) &amp; IF(ISBLANK(stand_md!CN4),"","_") &amp; UPPER(LEFT(stand_md!CN4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CN$3,1) &amp; RIGHT(plant_md!CN$3,LEN(plant_md!CN$3)-FIND(" ",plant_md!CN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CN$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CN$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CN$3,1) &amp; RIGHT(plant_md!CN$3,LEN(plant_md!CN$3)-FIND(" ",plant_md!CN$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CL3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CN$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CM5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CO2),"","_") &amp; UPPER(LEFT(stand_md!CO2,3)) &amp; IF(ISBLANK(stand_md!CO4),"","_") &amp; UPPER(LEFT(stand_md!CO4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CO$3,1) &amp; RIGHT(plant_md!CO$3,LEN(plant_md!CO$3)-FIND(" ",plant_md!CO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CO$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CO$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CO$3,1) &amp; RIGHT(plant_md!CO$3,LEN(plant_md!CO$3)-FIND(" ",plant_md!CO$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CM3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CO$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CN5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CP2),"","_") &amp; UPPER(LEFT(stand_md!CP2,3)) &amp; IF(ISBLANK(stand_md!CP4),"","_") &amp; UPPER(LEFT(stand_md!CP4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CP$3,1) &amp; RIGHT(plant_md!CP$3,LEN(plant_md!CP$3)-FIND(" ",plant_md!CP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CP$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CP$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CP$3,1) &amp; RIGHT(plant_md!CP$3,LEN(plant_md!CP$3)-FIND(" ",plant_md!CP$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CN3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CP$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CO5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CQ2),"","_") &amp; UPPER(LEFT(stand_md!CQ2,3)) &amp; IF(ISBLANK(stand_md!CQ4),"","_") &amp; UPPER(LEFT(stand_md!CQ4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CQ$3,1) &amp; RIGHT(plant_md!CQ$3,LEN(plant_md!CQ$3)-FIND(" ",plant_md!CQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CQ$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CQ$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CQ$3,1) &amp; RIGHT(plant_md!CQ$3,LEN(plant_md!CQ$3)-FIND(" ",plant_md!CQ$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CO3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CQ$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CP5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CR2),"","_") &amp; UPPER(LEFT(stand_md!CR2,3)) &amp; IF(ISBLANK(stand_md!CR4),"","_") &amp; UPPER(LEFT(stand_md!CR4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CR$3,1) &amp; RIGHT(plant_md!CR$3,LEN(plant_md!CR$3)-FIND(" ",plant_md!CR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CR$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CR$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CR$3,1) &amp; RIGHT(plant_md!CR$3,LEN(plant_md!CR$3)-FIND(" ",plant_md!CR$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CP3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CR$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CQ5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CS2),"","_") &amp; UPPER(LEFT(stand_md!CS2,3)) &amp; IF(ISBLANK(stand_md!CS4),"","_") &amp; UPPER(LEFT(stand_md!CS4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CS$3,1) &amp; RIGHT(plant_md!CS$3,LEN(plant_md!CS$3)-FIND(" ",plant_md!CS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CS$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CS$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CS$3,1) &amp; RIGHT(plant_md!CS$3,LEN(plant_md!CS$3)-FIND(" ",plant_md!CS$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CQ3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CS$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CR5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CT2),"","_") &amp; UPPER(LEFT(stand_md!CT2,3)) &amp; IF(ISBLANK(stand_md!CT4),"","_") &amp; UPPER(LEFT(stand_md!CT4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CT$3,1) &amp; RIGHT(plant_md!CT$3,LEN(plant_md!CT$3)-FIND(" ",plant_md!CT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CT$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CT$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CT$3,1) &amp; RIGHT(plant_md!CT$3,LEN(plant_md!CT$3)-FIND(" ",plant_md!CT$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CR3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CT$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CS5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CU2),"","_") &amp; UPPER(LEFT(stand_md!CU2,3)) &amp; IF(ISBLANK(stand_md!CU4),"","_") &amp; UPPER(LEFT(stand_md!CU4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CU$3,1) &amp; RIGHT(plant_md!CU$3,LEN(plant_md!CU$3)-FIND(" ",plant_md!CU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CU$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CU$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CU$3,1) &amp; RIGHT(plant_md!CU$3,LEN(plant_md!CU$3)-FIND(" ",plant_md!CU$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CS3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CU$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CT5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CV2),"","_") &amp; UPPER(LEFT(stand_md!CV2,3)) &amp; IF(ISBLANK(stand_md!CV4),"","_") &amp; UPPER(LEFT(stand_md!CV4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CV$3,1) &amp; RIGHT(plant_md!CV$3,LEN(plant_md!CV$3)-FIND(" ",plant_md!CV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CV$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CV$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CV$3,1) &amp; RIGHT(plant_md!CV$3,LEN(plant_md!CV$3)-FIND(" ",plant_md!CV$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CT3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CV$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CU5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CW2),"","_") &amp; UPPER(LEFT(stand_md!CW2,3)) &amp; IF(ISBLANK(stand_md!CW4),"","_") &amp; UPPER(LEFT(stand_md!CW4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CW$3,1) &amp; RIGHT(plant_md!CW$3,LEN(plant_md!CW$3)-FIND(" ",plant_md!CW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CW$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CW$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CW$3,1) &amp; RIGHT(plant_md!CW$3,LEN(plant_md!CW$3)-FIND(" ",plant_md!CW$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CU3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CW$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CV5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CX2),"","_") &amp; UPPER(LEFT(stand_md!CX2,3)) &amp; IF(ISBLANK(stand_md!CX4),"","_") &amp; UPPER(LEFT(stand_md!CX4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CX$3,1) &amp; RIGHT(plant_md!CX$3,LEN(plant_md!CX$3)-FIND(" ",plant_md!CX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CX$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CX$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CX$3,1) &amp; RIGHT(plant_md!CX$3,LEN(plant_md!CX$3)-FIND(" ",plant_md!CX$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CV3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CX$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
       <c r="CW5" s="86" t="str">
-        <f>IF(NOT(ISBLANK(plant_md!CY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!CY2),"","_") &amp; UPPER(LEFT(stand_md!CY2,3)) &amp; IF(ISBLANK(stand_md!CY4),"","_") &amp; UPPER(LEFT(stand_md!CY4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CY$3,1) &amp; RIGHT(plant_md!CY$3,LEN(plant_md!CY$3)-FIND(" ",plant_md!CY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CY$1,"Plant full code")</f>
+        <f>IF(NOT(ISBLANK(plant_md!CY$2)),UPPER(site_md!$D$4) &amp; "_" &amp; UPPER(LEFT(site_md!$D$3,3)) &amp; IF(ISBLANK(stand_md!$D$2),"","_") &amp; UPPER(LEFT(stand_md!$D$2,3)) &amp; IF(ISBLANK(stand_md!$D$4),"","_") &amp; UPPER(LEFT(stand_md!$D$4,3)) &amp; "_" &amp; LEFT(LEFT(plant_md!CY$3,1) &amp; RIGHT(plant_md!CY$3,LEN(plant_md!CY$3)-FIND(" ",plant_md!CY$3)),3) &amp; "_" &amp; IFERROR(IF(VLOOKUP(sapflow_hd!CW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flux density (per unit sapwood area).","Js",IF(VLOOKUP(sapflow_hd!CW3,plant_dic!$M$2:$N$14,2,FALSE)="sap flow (per tree).","Jt","Variable")),"Variable") &amp; "_" &amp;plant_md!CY$1,"Plant full code")</f>
         <v>Plant full code</v>
       </c>
     </row>
@@ -13417,7 +13417,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>

</xml_diff>